<commit_message>
UnclassifiedExamsConstriction and DifferentDayConstriction done.
</commit_message>
<xml_diff>
--- a/files/output/prueba.xlsx
+++ b/files/output/prueba.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="194">
   <si>
     <t>Curso</t>
   </si>
@@ -62,6 +62,93 @@
     <t>ID</t>
   </si>
   <si>
+    <t xml:space="preserve">GIISOF01-0-015 </t>
+  </si>
+  <si>
+    <t>SIW</t>
+  </si>
+  <si>
+    <t>Sistemas de Información para la Web</t>
+  </si>
+  <si>
+    <t>Teórico</t>
+  </si>
+  <si>
+    <t>No presencial</t>
+  </si>
+  <si>
+    <t>2:00:00</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>9:00:00</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-003</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>Ingeniería del Proceso Software</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>1:00:00</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-006</t>
+  </si>
+  <si>
+    <t>SSOO</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-005</t>
+  </si>
+  <si>
+    <t>ASLEPI</t>
+  </si>
+  <si>
+    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-004</t>
+  </si>
+  <si>
+    <t>DPPI</t>
+  </si>
+  <si>
+    <t>Dirección y Planificación de Proyectos Informáticos</t>
+  </si>
+  <si>
+    <t>2:30:00</t>
+  </si>
+  <si>
+    <t>18:30:00</t>
+  </si>
+  <si>
     <t>GIISOF01-1-003</t>
   </si>
   <si>
@@ -71,523 +158,442 @@
     <t>Empresa</t>
   </si>
   <si>
-    <t>Teórico</t>
-  </si>
-  <si>
-    <t>Presencial</t>
-  </si>
-  <si>
-    <t>2:30:00</t>
-  </si>
-  <si>
-    <t>lunes</t>
-  </si>
-  <si>
-    <t>9:00:00</t>
+    <t>21:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-004</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Cálculo</t>
+  </si>
+  <si>
+    <t>3:00:00</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-009 </t>
+  </si>
+  <si>
+    <t>Computación Numérica</t>
+  </si>
+  <si>
+    <t>Práctico</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-008</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Sistemas Inteligentes</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-007</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Introducción a la Programación</t>
+  </si>
+  <si>
+    <t>20:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-005 </t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>Sistemas Distribuidos e Internet</t>
+  </si>
+  <si>
+    <t>1:30:00</t>
+  </si>
+  <si>
+    <t>miércoles</t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-007</t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>Comunicación Persona-Máquina</t>
   </si>
   <si>
     <t>11:30:00</t>
   </si>
   <si>
-    <t>GIISOF01-4-004</t>
-  </si>
-  <si>
-    <t>DPPI</t>
-  </si>
-  <si>
-    <t>Dirección y Planificación de Proyectos Informáticos</t>
-  </si>
-  <si>
-    <t>No presencial</t>
+    <t>GIISOF01-1-001</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática (80)</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-004</t>
+  </si>
+  <si>
+    <t>TPP</t>
+  </si>
+  <si>
+    <t>Tecnología y Paradigmas de Programación</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-003</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Estructura de Datos</t>
+  </si>
+  <si>
+    <t>20:30:00</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-001</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Repositorios de Información</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-010</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Metodología de la Programación</t>
+  </si>
+  <si>
+    <t>18:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-002</t>
+  </si>
+  <si>
+    <t>SEW</t>
+  </si>
+  <si>
+    <t>Software y Estándares para la Web</t>
+  </si>
+  <si>
+    <t>19:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-008</t>
+  </si>
+  <si>
+    <t>FCR</t>
+  </si>
+  <si>
+    <t>Fundamentos de Computadores y Redes</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-016</t>
+  </si>
+  <si>
+    <t>SEV</t>
+  </si>
+  <si>
+    <t>Software de entretenimiento y videojuegos</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>0:30:00</t>
+  </si>
+  <si>
+    <t>12:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-003</t>
+  </si>
+  <si>
+    <t>CVVS</t>
+  </si>
+  <si>
+    <t>Calidad, Validación y Verificación del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-001</t>
+  </si>
+  <si>
+    <t>TEC</t>
+  </si>
+  <si>
+    <t>Tecnología Electrónica de Computadores</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-008</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Arquitectura del Software</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>19:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-010</t>
+  </si>
+  <si>
+    <t>IAE</t>
+  </si>
+  <si>
+    <t>Integración de aplicaciones empresariales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-002 </t>
+  </si>
+  <si>
+    <t>Presentación</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-002</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Ingeniería de Requisitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-001 </t>
+  </si>
+  <si>
+    <t>GIISOF01-0-011</t>
+  </si>
+  <si>
+    <t>IFA</t>
+  </si>
+  <si>
+    <t>Informática Forense y Auditoría</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-0-013 </t>
+  </si>
+  <si>
+    <t>SDM</t>
+  </si>
+  <si>
+    <t>Software para Dispositivos Móviles</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-005</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>Computabilidad</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-010</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Seguridad de Sistemas Informáticos</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-004</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Diseño del Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-007 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-008 </t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-008</t>
+  </si>
+  <si>
+    <t>BBDD</t>
+  </si>
+  <si>
+    <t>Bases de Datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-010 </t>
+  </si>
+  <si>
+    <t>GIISOF01-0-018</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Informática Audiovisual</t>
+  </si>
+  <si>
+    <t>15:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-005</t>
+  </si>
+  <si>
+    <t>OyE</t>
+  </si>
+  <si>
+    <t>Ondas y Electromagnetismo</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-002</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Arquitectura de Computadores</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-009</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-002</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Álgebra Lineal</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-009</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>14:00:00</t>
   </si>
   <si>
-    <t>GIISOF01-1-010</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>Metodología de la Programación</t>
-  </si>
-  <si>
-    <t>Práctico</t>
-  </si>
-  <si>
-    <t>3:00:00</t>
-  </si>
-  <si>
-    <t>15:00:00</t>
-  </si>
-  <si>
-    <t>18:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-009 </t>
-  </si>
-  <si>
-    <t>Computación Numérica</t>
-  </si>
-  <si>
-    <t>21:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-008</t>
-  </si>
-  <si>
-    <t>FCR</t>
-  </si>
-  <si>
-    <t>Fundamentos de Computadores y Redes</t>
-  </si>
-  <si>
-    <t>martes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-003</t>
-  </si>
-  <si>
-    <t>IPS</t>
-  </si>
-  <si>
-    <t>Ingeniería del Proceso Software</t>
-  </si>
-  <si>
-    <t>1:00:00</t>
-  </si>
-  <si>
-    <t>12:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-004</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>Diseño del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-004</t>
-  </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Cálculo</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-018</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>Informática Audiovisual</t>
-  </si>
-  <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
-    <t>Entrega</t>
-  </si>
-  <si>
-    <t>0:30:00</t>
-  </si>
-  <si>
-    <t>18:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-002</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Arquitectura de Computadores</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-005</t>
-  </si>
-  <si>
-    <t>Comp</t>
-  </si>
-  <si>
-    <t>Computabilidad</t>
-  </si>
-  <si>
-    <t>miércoles</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-016</t>
-  </si>
-  <si>
-    <t>SEV</t>
-  </si>
-  <si>
-    <t>Software de entretenimiento y videojuegos</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-002</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>Álgebra Lineal</t>
-  </si>
-  <si>
-    <t>15:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-009</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2:00:00</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-010</t>
-  </si>
-  <si>
-    <t>IAE</t>
-  </si>
-  <si>
-    <t>Integración de aplicaciones empresariales</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-011</t>
-  </si>
-  <si>
-    <t>IFA</t>
-  </si>
-  <si>
-    <t>Informática Forense y Auditoría</t>
-  </si>
-  <si>
-    <t>19:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-003</t>
-  </si>
-  <si>
-    <t>CVVS</t>
-  </si>
-  <si>
-    <t>Calidad, Validación y Verificación del Software</t>
-  </si>
-  <si>
-    <t>20:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-005</t>
-  </si>
-  <si>
-    <t>OyE</t>
-  </si>
-  <si>
-    <t>Ondas y Electromagnetismo</t>
-  </si>
-  <si>
-    <t>jueves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-007 </t>
-  </si>
-  <si>
-    <t>CPM</t>
-  </si>
-  <si>
-    <t>Comunicación Persona-Máquina</t>
+    <t>GIISOF01-0-017</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Software para Robots</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-005</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-006</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Administración de Sistemas y Redes</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-010</t>
+  </si>
+  <si>
+    <t>Alg</t>
+  </si>
+  <si>
+    <t>Algoritmia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-009 </t>
+  </si>
+  <si>
+    <t>DLP</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
+  </si>
+  <si>
+    <t>3:30:00</t>
+  </si>
+  <si>
+    <t>Autómatas y Matemáticas Discretas</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
+  </si>
+  <si>
+    <t>9:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-010 </t>
+  </si>
+  <si>
+    <t>GIISOF01-1-006</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Estadística</t>
   </si>
   <si>
     <t>GIISOF01-0-013</t>
-  </si>
-  <si>
-    <t>SDM</t>
-  </si>
-  <si>
-    <t>Software para Dispositivos Móviles</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-006</t>
-  </si>
-  <si>
-    <t>Est</t>
-  </si>
-  <si>
-    <t>Estadística</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-002 </t>
-  </si>
-  <si>
-    <t>SEW</t>
-  </si>
-  <si>
-    <t>Software y Estándares para la Web</t>
-  </si>
-  <si>
-    <t>19:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-010 </t>
-  </si>
-  <si>
-    <t>Alg</t>
-  </si>
-  <si>
-    <t>Algoritmia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-015 </t>
-  </si>
-  <si>
-    <t>SIW</t>
-  </si>
-  <si>
-    <t>Sistemas de Información para la Web</t>
-  </si>
-  <si>
-    <t>viernes</t>
-  </si>
-  <si>
-    <t>9:30:00</t>
-  </si>
-  <si>
-    <t>Autómatas y Matemáticas Discretas</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-008</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-004</t>
-  </si>
-  <si>
-    <t>TPP</t>
-  </si>
-  <si>
-    <t>Tecnología y Paradigmas de Programación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-004 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-013 </t>
-  </si>
-  <si>
-    <t>GIISOF01-4-005</t>
-  </si>
-  <si>
-    <t>ASLEPI</t>
-  </si>
-  <si>
-    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-003</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>Estructura de Datos</t>
-  </si>
-  <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-010 </t>
-  </si>
-  <si>
-    <t>SSI</t>
-  </si>
-  <si>
-    <t>Seguridad de Sistemas Informáticos</t>
-  </si>
-  <si>
-    <t>13:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-001</t>
-  </si>
-  <si>
-    <t>FI</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática (80)</t>
-  </si>
-  <si>
-    <t>17:00:00</t>
-  </si>
-  <si>
-    <t>20:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-002</t>
-  </si>
-  <si>
-    <t>IR</t>
-  </si>
-  <si>
-    <t>Ingeniería de Requisitos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-009 </t>
-  </si>
-  <si>
-    <t>DLP</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
-  </si>
-  <si>
-    <t>3:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-006</t>
-  </si>
-  <si>
-    <t>ASR</t>
-  </si>
-  <si>
-    <t>Administración de Sistemas y Redes</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-017</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>Software para Robots</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-007</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Introducción a la Programación</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-008</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Sistemas Inteligentes</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-009</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-007</t>
-  </si>
-  <si>
-    <t>Presentación</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-002</t>
-  </si>
-  <si>
-    <t>1:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-010</t>
-  </si>
-  <si>
-    <t>16:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-006</t>
-  </si>
-  <si>
-    <t>SSOO</t>
-  </si>
-  <si>
-    <t>Sistemas Operativos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-005 </t>
-  </si>
-  <si>
-    <t>SDI</t>
-  </si>
-  <si>
-    <t>Sistemas Distribuidos e Internet</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-010</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-005</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-008 </t>
-  </si>
-  <si>
-    <t>GIISOF01-2-001</t>
-  </si>
-  <si>
-    <t>TEC</t>
-  </si>
-  <si>
-    <t>Tecnología Electrónica de Computadores</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-001</t>
-  </si>
-  <si>
-    <t>RI</t>
-  </si>
-  <si>
-    <t>Repositorios de Información</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-008</t>
-  </si>
-  <si>
-    <t>BBDD</t>
-  </si>
-  <si>
-    <t>Bases de Datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-001 </t>
-  </si>
-  <si>
-    <t>13:00:00</t>
   </si>
 </sst>
 </file>
@@ -690,7 +696,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
@@ -714,7 +720,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="n">
-        <v>44.0</v>
+        <v>0.0</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -735,15 +741,15 @@
         <v>0.0</v>
       </c>
       <c r="P2" t="n">
-        <v>38.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -764,10 +770,10 @@
         <v>28</v>
       </c>
       <c r="I3" t="n">
-        <v>120.0</v>
+        <v>40.0</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K3" t="n">
         <v>44361.0</v>
@@ -779,45 +785,45 @@
         <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O3" t="n">
         <v>0.0</v>
       </c>
       <c r="P3" t="n">
-        <v>45.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B4" t="n">
         <v>2.0</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" t="n">
         <v>1.0</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I4" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K4" t="n">
         <v>44361.0</v>
@@ -826,48 +832,48 @@
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O4" t="n">
         <v>0.0</v>
       </c>
       <c r="P4" t="n">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="n">
         <v>2.0</v>
       </c>
       <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
       <c r="F5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="n">
-        <v>50.0</v>
+        <v>177.0</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K5" t="n">
         <v>44361.0</v>
@@ -876,7 +882,7 @@
         <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N5" t="s">
         <v>39</v>
@@ -885,12 +891,12 @@
         <v>0.0</v>
       </c>
       <c r="P5" t="n">
-        <v>49.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="B6" t="n">
         <v>2.0</v>
@@ -914,45 +920,45 @@
         <v>20</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0</v>
+        <v>120.0</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="K6" t="n">
-        <v>44362.0</v>
+        <v>44361.0</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="O6" t="n">
         <v>0.0</v>
       </c>
       <c r="P6" t="n">
-        <v>23.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B7" t="n">
         <v>1.0</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F7" t="n">
         <v>1.0</v>
@@ -961,22 +967,22 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I7" t="n">
-        <v>40.0</v>
+        <v>44.0</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K7" t="n">
-        <v>44362.0</v>
+        <v>44361.0</v>
       </c>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="N7" t="s">
         <v>48</v>
@@ -985,12 +991,12 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>11.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B8" t="n">
         <v>1.0</v>
@@ -1011,189 +1017,189 @@
         <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I8" t="n">
-        <v>150.0</v>
+        <v>140.0</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="K8" t="n">
         <v>44362.0</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="N8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O8" t="n">
         <v>0.0</v>
       </c>
       <c r="P8" t="n">
-        <v>2.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J9" t="s">
         <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
       </c>
       <c r="K9" t="n">
         <v>44362.0</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="O9" t="n">
         <v>0.0</v>
       </c>
       <c r="P9" t="n">
-        <v>40.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="B10" t="n">
         <v>1.0</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F10" t="n">
         <v>1.0</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0</v>
+        <v>103.0</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="K10" t="n">
         <v>44362.0</v>
       </c>
       <c r="L10" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O10" t="n">
         <v>0.0</v>
       </c>
       <c r="P10" t="n">
-        <v>36.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B11" t="n">
         <v>1.0</v>
       </c>
       <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
         <v>62</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>63</v>
       </c>
-      <c r="E11" t="s">
-        <v>64</v>
-      </c>
       <c r="F11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I11" t="n">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="K11" t="n">
         <v>44362.0</v>
       </c>
       <c r="L11" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N11" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="O11" t="n">
         <v>0.0</v>
       </c>
       <c r="P11" t="n">
-        <v>28.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -1205,87 +1211,87 @@
         <v>67</v>
       </c>
       <c r="F12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
       </c>
       <c r="I12" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="K12" t="n">
         <v>44363.0</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M12" t="s">
         <v>23</v>
       </c>
       <c r="N12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O12" t="n">
         <v>0.0</v>
       </c>
       <c r="P12" t="n">
-        <v>52.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B13" t="n">
         <v>1.0</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" t="n">
         <v>1.0</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0</v>
+        <v>84.0</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="K13" t="n">
         <v>44363.0</v>
       </c>
       <c r="L13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N13" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="O13" t="n">
         <v>0.0</v>
       </c>
       <c r="P13" t="n">
-        <v>54.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="14">
@@ -1296,101 +1302,101 @@
         <v>1.0</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F14" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I14" t="n">
-        <v>120.0</v>
+        <v>79.0</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K14" t="n">
         <v>44363.0</v>
       </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M14" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="N14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="O14" t="n">
         <v>0.0</v>
       </c>
       <c r="P14" t="n">
-        <v>56.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B15" t="n">
         <v>2.0</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F15" t="n">
         <v>1.0</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I15" t="n">
-        <v>70.0</v>
+        <v>61.0</v>
       </c>
       <c r="J15" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="K15" t="n">
         <v>44363.0</v>
       </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M15" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="N15" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="O15" t="n">
         <v>0.0</v>
       </c>
       <c r="P15" t="n">
-        <v>14.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B16" t="n">
         <v>1.0</v>
@@ -1408,101 +1414,101 @@
         <v>1.0</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
       </c>
       <c r="I16" t="n">
-        <v>3.0</v>
+        <v>62.0</v>
       </c>
       <c r="J16" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K16" t="n">
         <v>44363.0</v>
       </c>
       <c r="L16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M16" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="N16" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="O16" t="n">
         <v>0.0</v>
       </c>
       <c r="P16" t="n">
-        <v>25.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B17" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="F17" t="n">
         <v>1.0</v>
       </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
         <v>28</v>
       </c>
       <c r="I17" t="n">
-        <v>3.0</v>
+        <v>40.0</v>
       </c>
       <c r="J17" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K17" t="n">
-        <v>44363.0</v>
+        <v>44364.0</v>
       </c>
       <c r="L17" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="M17" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="N17" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="O17" t="n">
         <v>0.0</v>
       </c>
       <c r="P17" t="n">
-        <v>41.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B18" t="n">
         <v>1.0</v>
       </c>
       <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
         <v>89</v>
-      </c>
-      <c r="D18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" t="s">
-        <v>91</v>
       </c>
       <c r="F18" t="n">
         <v>1.0</v>
@@ -1514,28 +1520,28 @@
         <v>20</v>
       </c>
       <c r="I18" t="n">
-        <v>45.0</v>
+        <v>67.0</v>
       </c>
       <c r="J18" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="K18" t="n">
-        <v>44363.0</v>
+        <v>44364.0</v>
       </c>
       <c r="L18" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="M18" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="N18" t="s">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="O18" t="n">
         <v>0.0</v>
       </c>
       <c r="P18" t="n">
-        <v>30.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="19">
@@ -1546,246 +1552,246 @@
         <v>2.0</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F19" t="n">
         <v>1.0</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I19" t="n">
-        <v>150.0</v>
+        <v>50.0</v>
       </c>
       <c r="J19" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="K19" t="n">
         <v>44364.0</v>
       </c>
       <c r="L19" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="O19" t="n">
         <v>0.0</v>
       </c>
       <c r="P19" t="n">
-        <v>26.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B20" t="n">
         <v>1.0</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F20" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I20" t="n">
         <v>0.0</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="K20" t="n">
         <v>44364.0</v>
       </c>
       <c r="L20" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="M20" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="N20" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="O20" t="n">
         <v>0.0</v>
       </c>
       <c r="P20" t="n">
-        <v>42.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B21" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" t="s">
         <v>100</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" t="n">
+        <v>44365.0</v>
+      </c>
+      <c r="L21" t="s">
         <v>101</v>
       </c>
-      <c r="E21" t="s">
-        <v>102</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" t="s">
-        <v>59</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>60</v>
-      </c>
-      <c r="K21" t="n">
-        <v>44364.0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>96</v>
-      </c>
       <c r="M21" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="N21" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="O21" t="n">
         <v>0.0</v>
       </c>
       <c r="P21" t="n">
-        <v>3.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B22" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
         <v>103</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>104</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G22" t="s">
         <v>105</v>
       </c>
-      <c r="F22" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G22" t="s">
-        <v>19</v>
-      </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="I22" t="n">
-        <v>183.0</v>
+        <v>0.0</v>
       </c>
       <c r="J22" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="K22" t="n">
-        <v>44364.0</v>
+        <v>44365.0</v>
       </c>
       <c r="L22" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="M22" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="N22" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="O22" t="n">
         <v>0.0</v>
       </c>
       <c r="P22" t="n">
-        <v>47.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B23" t="n">
         <v>1.0</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" t="n">
+        <v>44365.0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>101</v>
+      </c>
+      <c r="M23" t="s">
         <v>108</v>
       </c>
-      <c r="F23" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>60</v>
-      </c>
-      <c r="K23" t="n">
-        <v>44364.0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>96</v>
-      </c>
-      <c r="M23" t="s">
-        <v>61</v>
-      </c>
       <c r="N23" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="O23" t="n">
         <v>0.0</v>
       </c>
       <c r="P23" t="n">
-        <v>34.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="24">
@@ -1793,40 +1799,40 @@
         <v>2.0</v>
       </c>
       <c r="B24" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F24" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H24" t="s">
         <v>20</v>
       </c>
       <c r="I24" t="n">
-        <v>30.0</v>
+        <v>8.0</v>
       </c>
       <c r="J24" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="K24" t="n">
-        <v>44364.0</v>
+        <v>44365.0</v>
       </c>
       <c r="L24" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="M24" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="N24" t="s">
         <v>39</v>
@@ -1835,124 +1841,124 @@
         <v>0.0</v>
       </c>
       <c r="P24" t="n">
-        <v>46.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B25" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E25" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="I25" t="n">
         <v>0.0</v>
       </c>
       <c r="J25" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="K25" t="n">
         <v>44365.0</v>
       </c>
       <c r="L25" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="N25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O25" t="n">
         <v>0.0</v>
       </c>
       <c r="P25" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B26" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="F26" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G26" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I26" t="n">
-        <v>70.0</v>
+        <v>62.0</v>
       </c>
       <c r="J26" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="K26" t="n">
         <v>44365.0</v>
       </c>
       <c r="L26" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N26" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="O26" t="n">
         <v>0.0</v>
       </c>
       <c r="P26" t="n">
-        <v>32.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B27" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E27" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F27" t="n">
         <v>1.0</v>
@@ -1961,86 +1967,86 @@
         <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="J27" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="K27" t="n">
         <v>44365.0</v>
       </c>
       <c r="L27" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M27" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="N27" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="O27" t="n">
         <v>0.0</v>
       </c>
       <c r="P27" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B28" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D28" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" t="s">
         <v>124</v>
       </c>
-      <c r="F28" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G28" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" t="s">
-        <v>20</v>
-      </c>
       <c r="I28" t="n">
-        <v>61.0</v>
+        <v>0.0</v>
       </c>
       <c r="J28" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="K28" t="n">
-        <v>44365.0</v>
+        <v>44368.0</v>
       </c>
       <c r="L28" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="M28" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="N28" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O28" t="n">
         <v>0.0</v>
       </c>
       <c r="P28" t="n">
-        <v>7.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B29" t="n">
         <v>1.0</v>
@@ -2049,110 +2055,110 @@
         <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="F29" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I29" t="n">
-        <v>79.0</v>
+        <v>90.0</v>
       </c>
       <c r="J29" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="K29" t="n">
-        <v>44365.0</v>
+        <v>44368.0</v>
       </c>
       <c r="L29" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="M29" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N29" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="O29" t="n">
         <v>0.0</v>
       </c>
       <c r="P29" t="n">
-        <v>37.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B30" t="n">
         <v>1.0</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="F30" t="n">
         <v>2.0</v>
       </c>
       <c r="G30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H30" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="I30" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="J30" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="K30" t="n">
-        <v>44365.0</v>
+        <v>44368.0</v>
       </c>
       <c r="L30" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="M30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N30" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="O30" t="n">
         <v>0.0</v>
       </c>
       <c r="P30" t="n">
-        <v>13.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="B31" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D31" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F31" t="n">
         <v>1.0</v>
@@ -2161,63 +2167,63 @@
         <v>19</v>
       </c>
       <c r="H31" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I31" t="n">
-        <v>177.0</v>
+        <v>3.0</v>
       </c>
       <c r="J31" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="K31" t="n">
-        <v>44365.0</v>
+        <v>44368.0</v>
       </c>
       <c r="L31" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="M31" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="N31" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="O31" t="n">
         <v>0.0</v>
       </c>
       <c r="P31" t="n">
-        <v>53.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B32" t="n">
         <v>1.0</v>
       </c>
       <c r="C32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E32" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F32" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="H32" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="I32" t="n">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="J32" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="K32" t="n">
         <v>44368.0</v>
@@ -2226,48 +2232,48 @@
         <v>22</v>
       </c>
       <c r="M32" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="N32" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="O32" t="n">
         <v>0.0</v>
       </c>
       <c r="P32" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B33" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E33" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F33" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G33" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H33" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I33" t="n">
-        <v>71.0</v>
+        <v>70.0</v>
       </c>
       <c r="J33" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="K33" t="n">
         <v>44368.0</v>
@@ -2276,24 +2282,24 @@
         <v>22</v>
       </c>
       <c r="M33" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
       <c r="N33" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="O33" t="n">
         <v>0.0</v>
       </c>
       <c r="P33" t="n">
-        <v>51.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B34" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C34" t="s">
         <v>138</v>
@@ -2305,104 +2311,104 @@
         <v>140</v>
       </c>
       <c r="F34" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H34" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I34" t="n">
-        <v>79.0</v>
+        <v>116.0</v>
       </c>
       <c r="J34" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="K34" t="n">
-        <v>44368.0</v>
+        <v>44369.0</v>
       </c>
       <c r="L34" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="M34" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="O34" t="n">
         <v>0.0</v>
       </c>
       <c r="P34" t="n">
-        <v>29.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B35" t="n">
         <v>1.0</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="F35" t="n">
         <v>1.0</v>
       </c>
       <c r="G35" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I35" t="n">
-        <v>62.0</v>
+        <v>80.0</v>
       </c>
       <c r="J35" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K35" t="n">
-        <v>44368.0</v>
+        <v>44369.0</v>
       </c>
       <c r="L35" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="M35" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="N35" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="O35" t="n">
         <v>0.0</v>
       </c>
       <c r="P35" t="n">
-        <v>35.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B36" t="n">
         <v>1.0</v>
       </c>
       <c r="C36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" t="s">
         <v>143</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>144</v>
-      </c>
-      <c r="E36" t="s">
-        <v>145</v>
       </c>
       <c r="F36" t="n">
         <v>1.0</v>
@@ -2411,81 +2417,81 @@
         <v>19</v>
       </c>
       <c r="H36" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I36" t="n">
-        <v>90.0</v>
+        <v>150.0</v>
       </c>
       <c r="J36" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K36" t="n">
         <v>44369.0</v>
       </c>
       <c r="L36" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M36" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="N36" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="O36" t="n">
         <v>0.0</v>
       </c>
       <c r="P36" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B37" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="F37" t="n">
         <v>2.0</v>
       </c>
       <c r="G37" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H37" t="s">
         <v>20</v>
       </c>
       <c r="I37" t="n">
-        <v>89.0</v>
+        <v>0.0</v>
       </c>
       <c r="J37" t="s">
-        <v>149</v>
+        <v>52</v>
       </c>
       <c r="K37" t="n">
         <v>44369.0</v>
       </c>
       <c r="L37" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M37" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="N37" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="O37" t="n">
         <v>0.0</v>
       </c>
       <c r="P37" t="n">
-        <v>58.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="38">
@@ -2493,249 +2499,249 @@
         <v>3.0</v>
       </c>
       <c r="B38" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D38" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E38" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F38" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H38" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0</v>
+        <v>79.0</v>
       </c>
       <c r="J38" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K38" t="n">
         <v>44369.0</v>
       </c>
       <c r="L38" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M38" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="N38" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
       <c r="O38" t="n">
         <v>0.0</v>
       </c>
       <c r="P38" t="n">
-        <v>5.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B39" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E39" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="F39" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G39" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
+        <v>124</v>
       </c>
       <c r="I39" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="J39" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K39" t="n">
-        <v>44369.0</v>
+        <v>44370.0</v>
       </c>
       <c r="L39" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="M39" t="s">
-        <v>153</v>
+        <v>23</v>
       </c>
       <c r="N39" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="O39" t="n">
         <v>0.0</v>
       </c>
       <c r="P39" t="n">
-        <v>4.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B40" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C40" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E40" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F40" t="n">
         <v>1.0</v>
       </c>
       <c r="G40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H40" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0</v>
+        <v>71.0</v>
       </c>
       <c r="J40" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="K40" t="n">
-        <v>44369.0</v>
+        <v>44370.0</v>
       </c>
       <c r="L40" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="M40" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="N40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O40" t="n">
         <v>0.0</v>
       </c>
       <c r="P40" t="n">
-        <v>50.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B41" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E41" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F41" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G41" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I41" t="n">
-        <v>50.0</v>
+        <v>71.0</v>
       </c>
       <c r="J41" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="K41" t="n">
         <v>44370.0</v>
       </c>
       <c r="L41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M41" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="N41" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="O41" t="n">
         <v>0.0</v>
       </c>
       <c r="P41" t="n">
-        <v>44.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="B42" t="n">
         <v>1.0</v>
       </c>
       <c r="C42" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
       </c>
       <c r="G42" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="H42" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="I42" t="n">
-        <v>103.0</v>
+        <v>0.0</v>
       </c>
       <c r="J42" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="K42" t="n">
         <v>44370.0</v>
       </c>
       <c r="L42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M42" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="N42" t="s">
-        <v>29</v>
+        <v>156</v>
       </c>
       <c r="O42" t="n">
         <v>0.0</v>
       </c>
       <c r="P42" t="n">
-        <v>6.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="43">
@@ -2746,13 +2752,13 @@
         <v>2.0</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
       <c r="F43" t="n">
         <v>1.0</v>
@@ -2761,48 +2767,48 @@
         <v>19</v>
       </c>
       <c r="H43" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I43" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c r="J43" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="K43" t="n">
         <v>44370.0</v>
       </c>
       <c r="L43" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M43" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="N43" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="O43" t="n">
         <v>0.0</v>
       </c>
       <c r="P43" t="n">
-        <v>18.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B44" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="D44" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="E44" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="F44" t="n">
         <v>1.0</v>
@@ -2814,145 +2820,145 @@
         <v>28</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0</v>
+        <v>150.0</v>
       </c>
       <c r="J44" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="K44" t="n">
-        <v>44370.0</v>
+        <v>44371.0</v>
       </c>
       <c r="L44" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="M44" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="N44" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="O44" t="n">
         <v>0.0</v>
       </c>
       <c r="P44" t="n">
-        <v>19.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B45" t="n">
         <v>1.0</v>
       </c>
       <c r="C45" t="s">
-        <v>164</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="F45" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G45" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="H45" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="I45" t="n">
-        <v>84.0</v>
+        <v>0.0</v>
       </c>
       <c r="J45" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="K45" t="n">
-        <v>44370.0</v>
+        <v>44371.0</v>
       </c>
       <c r="L45" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="M45" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="N45" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="O45" t="n">
         <v>0.0</v>
       </c>
       <c r="P45" t="n">
-        <v>16.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B46" t="n">
         <v>1.0</v>
       </c>
       <c r="C46" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="D46" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
       <c r="E46" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="F46" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G46" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H46" t="s">
-        <v>165</v>
+        <v>28</v>
       </c>
       <c r="I46" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="J46" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="K46" t="n">
         <v>44371.0</v>
       </c>
       <c r="L46" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="M46" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="N46" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="O46" t="n">
         <v>0.0</v>
       </c>
       <c r="P46" t="n">
-        <v>43.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B47" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C47" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="F47" t="n">
         <v>1.0</v>
@@ -2964,45 +2970,45 @@
         <v>28</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="J47" t="s">
-        <v>167</v>
+        <v>52</v>
       </c>
       <c r="K47" t="n">
         <v>44371.0</v>
       </c>
       <c r="L47" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="M47" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="N47" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="O47" t="n">
         <v>0.0</v>
       </c>
       <c r="P47" t="n">
-        <v>33.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B48" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="E48" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="F48" t="n">
         <v>1.0</v>
@@ -3011,48 +3017,48 @@
         <v>19</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I48" t="n">
-        <v>116.0</v>
+        <v>120.0</v>
       </c>
       <c r="J48" t="s">
-        <v>167</v>
+        <v>52</v>
       </c>
       <c r="K48" t="n">
         <v>44371.0</v>
       </c>
       <c r="L48" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="M48" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="N48" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
       <c r="O48" t="n">
         <v>0.0</v>
       </c>
       <c r="P48" t="n">
-        <v>27.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B49" t="n">
         <v>2.0</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D49" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E49" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F49" t="n">
         <v>1.0</v>
@@ -3061,31 +3067,31 @@
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I49" t="n">
-        <v>40.0</v>
+        <v>70.0</v>
       </c>
       <c r="J49" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="K49" t="n">
-        <v>44371.0</v>
+        <v>44372.0</v>
       </c>
       <c r="L49" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="M49" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="N49" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="O49" t="n">
         <v>0.0</v>
       </c>
       <c r="P49" t="n">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="50">
@@ -3093,66 +3099,66 @@
         <v>3.0</v>
       </c>
       <c r="B50" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="E50" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="F50" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G50" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="H50" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="I50" t="n">
         <v>0.0</v>
       </c>
       <c r="J50" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="K50" t="n">
-        <v>44371.0</v>
+        <v>44372.0</v>
       </c>
       <c r="L50" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="M50" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="N50" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="O50" t="n">
         <v>0.0</v>
       </c>
       <c r="P50" t="n">
-        <v>48.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B51" t="n">
         <v>1.0</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="D51" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E51" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="F51" t="n">
         <v>1.0</v>
@@ -3161,186 +3167,186 @@
         <v>19</v>
       </c>
       <c r="H51" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I51" t="n">
-        <v>80.0</v>
+        <v>60.0</v>
       </c>
       <c r="J51" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="K51" t="n">
-        <v>44371.0</v>
+        <v>44372.0</v>
       </c>
       <c r="L51" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="M51" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="N51" t="s">
-        <v>39</v>
+        <v>170</v>
       </c>
       <c r="O51" t="n">
         <v>0.0</v>
       </c>
       <c r="P51" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B52" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C52" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F52" t="n">
         <v>1.0</v>
       </c>
       <c r="G52" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="H52" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="I52" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J52" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="K52" t="n">
         <v>44372.0</v>
       </c>
       <c r="L52" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M52" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N52" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="O52" t="n">
         <v>0.0</v>
       </c>
       <c r="P52" t="n">
-        <v>31.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B53" t="n">
         <v>2.0</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="E53" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="F53" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G53" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H53" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I53" t="n">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="J53" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="K53" t="n">
         <v>44372.0</v>
       </c>
       <c r="L53" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M53" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="N53" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="O53" t="n">
         <v>0.0</v>
       </c>
       <c r="P53" t="n">
-        <v>61.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B54" t="n">
         <v>2.0</v>
       </c>
       <c r="C54" t="s">
+        <v>175</v>
+      </c>
+      <c r="D54" t="s">
+        <v>176</v>
+      </c>
+      <c r="E54" t="s">
         <v>177</v>
       </c>
-      <c r="D54" t="s">
-        <v>111</v>
-      </c>
-      <c r="E54" t="s">
-        <v>112</v>
-      </c>
       <c r="F54" t="n">
         <v>1.0</v>
       </c>
       <c r="G54" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="H54" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="I54" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="J54" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="K54" t="n">
         <v>44372.0</v>
       </c>
       <c r="L54" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M54" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="N54" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="O54" t="n">
         <v>0.0</v>
       </c>
       <c r="P54" t="n">
-        <v>24.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B55" t="n">
         <v>2.0</v>
@@ -3349,10 +3355,10 @@
         <v>178</v>
       </c>
       <c r="D55" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E55" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F55" t="n">
         <v>1.0</v>
@@ -3361,31 +3367,31 @@
         <v>19</v>
       </c>
       <c r="H55" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I55" t="n">
-        <v>40.0</v>
+        <v>100.0</v>
       </c>
       <c r="J55" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="K55" t="n">
         <v>44372.0</v>
       </c>
       <c r="L55" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M55" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="N55" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O55" t="n">
         <v>0.0</v>
       </c>
       <c r="P55" t="n">
-        <v>15.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="56">
@@ -3396,28 +3402,28 @@
         <v>2.0</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D56" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="E56" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F56" t="n">
         <v>2.0</v>
       </c>
       <c r="G56" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H56" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I56" t="n">
         <v>11.0</v>
       </c>
       <c r="J56" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="K56" t="n">
         <v>44375.0</v>
@@ -3429,7 +3435,7 @@
         <v>23</v>
       </c>
       <c r="N56" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="O56" t="n">
         <v>0.0</v>
@@ -3440,34 +3446,34 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B57" t="n">
         <v>2.0</v>
       </c>
       <c r="C57" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="E57" t="s">
-        <v>121</v>
+        <v>185</v>
       </c>
       <c r="F57" t="n">
         <v>2.0</v>
       </c>
       <c r="G57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H57" t="s">
-        <v>165</v>
+        <v>28</v>
       </c>
       <c r="I57" t="n">
-        <v>0.0</v>
+        <v>70.0</v>
       </c>
       <c r="J57" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="K57" t="n">
         <v>44375.0</v>
@@ -3476,24 +3482,24 @@
         <v>22</v>
       </c>
       <c r="M57" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="N57" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="O57" t="n">
         <v>0.0</v>
       </c>
       <c r="P57" t="n">
-        <v>22.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B58" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C58" t="s">
         <v>181</v>
@@ -3502,22 +3508,22 @@
         <v>182</v>
       </c>
       <c r="E58" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F58" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G58" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="H58" t="s">
         <v>28</v>
       </c>
       <c r="I58" t="n">
-        <v>8.0</v>
+        <v>89.0</v>
       </c>
       <c r="J58" t="s">
-        <v>47</v>
+        <v>184</v>
       </c>
       <c r="K58" t="n">
         <v>44375.0</v>
@@ -3526,33 +3532,33 @@
         <v>22</v>
       </c>
       <c r="M58" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N58" t="s">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="O58" t="n">
         <v>0.0</v>
       </c>
       <c r="P58" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B59" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C59" t="s">
-        <v>184</v>
+        <v>98</v>
       </c>
       <c r="D59" t="s">
-        <v>185</v>
+        <v>99</v>
       </c>
       <c r="E59" t="s">
-        <v>186</v>
+        <v>100</v>
       </c>
       <c r="F59" t="n">
         <v>1.0</v>
@@ -3564,10 +3570,10 @@
         <v>28</v>
       </c>
       <c r="I59" t="n">
-        <v>67.0</v>
+        <v>0.0</v>
       </c>
       <c r="J59" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K59" t="n">
         <v>44375.0</v>
@@ -3576,66 +3582,66 @@
         <v>22</v>
       </c>
       <c r="M59" t="s">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="N59" t="s">
-        <v>141</v>
+        <v>48</v>
       </c>
       <c r="O59" t="n">
         <v>0.0</v>
       </c>
       <c r="P59" t="n">
-        <v>9.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B60" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C60" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
       <c r="D60" t="s">
+        <v>95</v>
+      </c>
+      <c r="E60" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G60" t="s">
+        <v>105</v>
+      </c>
+      <c r="H60" t="s">
+        <v>106</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>107</v>
+      </c>
+      <c r="K60" t="n">
+        <v>44376.0</v>
+      </c>
+      <c r="L60" t="s">
+        <v>53</v>
+      </c>
+      <c r="M60" t="s">
+        <v>23</v>
+      </c>
+      <c r="N60" t="s">
         <v>188</v>
       </c>
-      <c r="E60" t="s">
-        <v>189</v>
-      </c>
-      <c r="F60" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G60" t="s">
-        <v>19</v>
-      </c>
-      <c r="H60" t="s">
-        <v>20</v>
-      </c>
-      <c r="I60" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="J60" t="s">
-        <v>34</v>
-      </c>
-      <c r="K60" t="n">
-        <v>44375.0</v>
-      </c>
-      <c r="L60" t="s">
-        <v>22</v>
-      </c>
-      <c r="M60" t="s">
-        <v>141</v>
-      </c>
-      <c r="N60" t="s">
-        <v>142</v>
-      </c>
       <c r="O60" t="n">
         <v>0.0</v>
       </c>
       <c r="P60" t="n">
-        <v>39.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="61">
@@ -3646,25 +3652,25 @@
         <v>2.0</v>
       </c>
       <c r="C61" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D61" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F61" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G61" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H61" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I61" t="n">
-        <v>71.0</v>
+        <v>30.0</v>
       </c>
       <c r="J61" t="s">
         <v>21</v>
@@ -3673,119 +3679,119 @@
         <v>44376.0</v>
       </c>
       <c r="L61" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M61" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="N61" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="O61" t="n">
         <v>0.0</v>
       </c>
       <c r="P61" t="n">
-        <v>55.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B62" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C62" t="s">
         <v>190</v>
       </c>
       <c r="D62" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="E62" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="F62" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G62" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H62" t="s">
         <v>28</v>
       </c>
       <c r="I62" t="n">
-        <v>8.0</v>
+        <v>183.0</v>
       </c>
       <c r="J62" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K62" t="n">
         <v>44376.0</v>
       </c>
       <c r="L62" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M62" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="N62" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="O62" t="n">
         <v>0.0</v>
       </c>
       <c r="P62" t="n">
-        <v>59.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C63" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="D63" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="E63" t="s">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="F63" t="n">
         <v>1.0</v>
       </c>
       <c r="G63" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="H63" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="I63" t="n">
         <v>0.0</v>
       </c>
       <c r="J63" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="K63" t="n">
         <v>44376.0</v>
       </c>
       <c r="L63" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M63" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="N63" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="O63" t="n">
         <v>0.0</v>
       </c>
       <c r="P63" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Whole new approach to parse constrictions so it is clearer for the user when writting the excel.
</commit_message>
<xml_diff>
--- a/files/output/prueba.xlsx
+++ b/files/output/prueba.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="188">
   <si>
     <t>Curso</t>
   </si>
@@ -62,244 +62,511 @@
     <t>ID</t>
   </si>
   <si>
+    <t>GIISOF01-0-010</t>
+  </si>
+  <si>
+    <t>IAE</t>
+  </si>
+  <si>
+    <t>Integración de aplicaciones empresariales</t>
+  </si>
+  <si>
+    <t>Teórico</t>
+  </si>
+  <si>
+    <t>No presencial</t>
+  </si>
+  <si>
+    <t>1:00:00</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>9:00:00</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-0-015 </t>
+  </si>
+  <si>
+    <t>SIW</t>
+  </si>
+  <si>
+    <t>Sistemas de Información para la Web</t>
+  </si>
+  <si>
+    <t>2:00:00</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-006</t>
+  </si>
+  <si>
+    <t>SSOO</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-002 </t>
+  </si>
+  <si>
+    <t>SEW</t>
+  </si>
+  <si>
+    <t>Software y Estándares para la Web</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Presentación</t>
+  </si>
+  <si>
+    <t>3:00:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>18:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-002</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Ingeniería de Requisitos</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>0:30:00</t>
+  </si>
+  <si>
+    <t>12:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-001 </t>
+  </si>
+  <si>
+    <t>TEC</t>
+  </si>
+  <si>
+    <t>Tecnología Electrónica de Computadores</t>
+  </si>
+  <si>
+    <t>Práctico</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-001</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Repositorios de Información</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-002</t>
+  </si>
+  <si>
+    <t>1:30:00</t>
+  </si>
+  <si>
+    <t>miércoles</t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-005</t>
+  </si>
+  <si>
+    <t>ASLEPI</t>
+  </si>
+  <si>
+    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-002</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Arquitectura de Computadores</t>
+  </si>
+  <si>
+    <t>2:30:00</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-002</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Álgebra Lineal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-0-013 </t>
+  </si>
+  <si>
+    <t>SDM</t>
+  </si>
+  <si>
+    <t>Software para Dispositivos Móviles</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>9:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-010</t>
+  </si>
+  <si>
+    <t>Alg</t>
+  </si>
+  <si>
+    <t>Algoritmia</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-007</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Introducción a la Programación</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-010 </t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Seguridad de Sistemas Informáticos</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
     <t>GIISOF01-0-013</t>
   </si>
   <si>
-    <t>SDM</t>
-  </si>
-  <si>
-    <t>Software para Dispositivos Móviles</t>
-  </si>
-  <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
-    <t>Entrega</t>
-  </si>
-  <si>
-    <t>0:30:00</t>
-  </si>
-  <si>
-    <t>lunes</t>
-  </si>
-  <si>
-    <t>9:00:00</t>
-  </si>
-  <si>
-    <t>9:30:00</t>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-005 </t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>Sistemas Distribuidos e Internet</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-001</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-006</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Estadística</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-008</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Sistemas Inteligentes</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-008</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Arquitectura del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-010</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Metodología de la Programación</t>
+  </si>
+  <si>
+    <t>15:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-008</t>
+  </si>
+  <si>
+    <t>BBDD</t>
+  </si>
+  <si>
+    <t>Bases de Datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-009 </t>
+  </si>
+  <si>
+    <t>DLP</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
+  </si>
+  <si>
+    <t>3:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-003</t>
+  </si>
+  <si>
+    <t>CVVS</t>
+  </si>
+  <si>
+    <t>Calidad, Validación y Verificación del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-011</t>
+  </si>
+  <si>
+    <t>IFA</t>
+  </si>
+  <si>
+    <t>Informática Forense y Auditoría</t>
+  </si>
+  <si>
+    <t>18:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-008</t>
+  </si>
+  <si>
+    <t>FCR</t>
+  </si>
+  <si>
+    <t>Fundamentos de Computadores y Redes</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-009</t>
+  </si>
+  <si>
+    <t>Computación Numérica</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-017</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Software para Robots</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-005</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-003</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Estructura de Datos</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-005</t>
+  </si>
+  <si>
+    <t>OyE</t>
+  </si>
+  <si>
+    <t>Ondas y Electromagnetismo</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-018</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Informática Audiovisual</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-007</t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>Comunicación Persona-Máquina</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-004</t>
+  </si>
+  <si>
+    <t>DPPI</t>
+  </si>
+  <si>
+    <t>Dirección y Planificación de Proyectos Informáticos</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-010 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-009 </t>
+  </si>
+  <si>
+    <t>GIISOF01-1-009</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>GIISOF01-0-016</t>
+  </si>
+  <si>
+    <t>SEV</t>
+  </si>
+  <si>
+    <t>Software de entretenimiento y videojuegos</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-004</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Cálculo</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-004</t>
+  </si>
+  <si>
+    <t>TPP</t>
+  </si>
+  <si>
+    <t>Tecnología y Paradigmas de Programación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-008 </t>
+  </si>
+  <si>
+    <t>Autómatas y Matemáticas Discretas</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-001</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática</t>
   </si>
   <si>
     <t xml:space="preserve">GIISOF01-2-007 </t>
   </si>
   <si>
-    <t>CPM</t>
-  </si>
-  <si>
-    <t>Comunicación Persona-Máquina</t>
-  </si>
-  <si>
-    <t>Práctico</t>
-  </si>
-  <si>
-    <t>No presencial</t>
-  </si>
-  <si>
-    <t>3:00:00</t>
-  </si>
-  <si>
-    <t>12:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-002 </t>
-  </si>
-  <si>
-    <t>SEW</t>
-  </si>
-  <si>
-    <t>Software y Estándares para la Web</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-001</t>
-  </si>
-  <si>
-    <t>FI</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática</t>
-  </si>
-  <si>
-    <t>Teórico</t>
-  </si>
-  <si>
-    <t>Presencial</t>
-  </si>
-  <si>
-    <t>2:00:00</t>
-  </si>
-  <si>
-    <t>15:00:00</t>
-  </si>
-  <si>
-    <t>17:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-005 </t>
-  </si>
-  <si>
-    <t>SDI</t>
-  </si>
-  <si>
-    <t>Sistemas Distribuidos e Internet</t>
-  </si>
-  <si>
-    <t>1:30:00</t>
-  </si>
-  <si>
-    <t>martes</t>
-  </si>
-  <si>
-    <t>10:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-018</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>Informática Audiovisual</t>
-  </si>
-  <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-009</t>
-  </si>
-  <si>
-    <t>Computación Numérica</t>
-  </si>
-  <si>
-    <t>14:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-006</t>
-  </si>
-  <si>
-    <t>SSOO</t>
-  </si>
-  <si>
-    <t>Sistemas Operativos</t>
-  </si>
-  <si>
-    <t>18:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-004</t>
-  </si>
-  <si>
-    <t>DPPI</t>
-  </si>
-  <si>
-    <t>Dirección y Planificación de Proyectos Informáticos</t>
-  </si>
-  <si>
-    <t>2:30:00</t>
-  </si>
-  <si>
-    <t>miércoles</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-002</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>Álgebra Lineal</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-010</t>
-  </si>
-  <si>
-    <t>SSI</t>
-  </si>
-  <si>
-    <t>Seguridad de Sistemas Informáticos</t>
-  </si>
-  <si>
-    <t>16:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-002</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Arquitectura de Computadores</t>
-  </si>
-  <si>
-    <t>19:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-002</t>
-  </si>
-  <si>
-    <t>jueves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-015 </t>
-  </si>
-  <si>
-    <t>SIW</t>
-  </si>
-  <si>
-    <t>Sistemas de Información para la Web</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-001</t>
-  </si>
-  <si>
-    <t>TEC</t>
-  </si>
-  <si>
-    <t>Tecnología Electrónica de Computadores</t>
-  </si>
-  <si>
-    <t>1:00:00</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-003</t>
-  </si>
-  <si>
-    <t>CVVS</t>
-  </si>
-  <si>
-    <t>Calidad, Validación y Verificación del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-002</t>
-  </si>
-  <si>
-    <t>IR</t>
-  </si>
-  <si>
-    <t>Ingeniería de Requisitos</t>
-  </si>
-  <si>
-    <t>viernes</t>
+    <t>GIISOF01-3-004</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Diseño del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-003</t>
+  </si>
+  <si>
+    <t>Emp</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-006</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Administración de Sistemas y Redes</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-003</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>Ingeniería del Proceso Software</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática (80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-004 </t>
   </si>
   <si>
     <t>GIISOF01-2-005</t>
@@ -309,288 +576,6 @@
   </si>
   <si>
     <t>Computabilidad</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-003</t>
-  </si>
-  <si>
-    <t>Emp</t>
-  </si>
-  <si>
-    <t>Empresa</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-010 </t>
-  </si>
-  <si>
-    <t>20:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-008</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Sistemas Inteligentes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-005</t>
-  </si>
-  <si>
-    <t>13:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-007</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-008</t>
-  </si>
-  <si>
-    <t>FCR</t>
-  </si>
-  <si>
-    <t>Fundamentos de Computadores y Redes</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-017</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>Software para Robots</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-010</t>
-  </si>
-  <si>
-    <t>Alg</t>
-  </si>
-  <si>
-    <t>Algoritmia</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-009</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>Autómatas y Matemáticas Discretas</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-001</t>
-  </si>
-  <si>
-    <t>RI</t>
-  </si>
-  <si>
-    <t>Repositorios de Información</t>
-  </si>
-  <si>
-    <t>15:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-008 </t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>Presentación</t>
-  </si>
-  <si>
-    <t>10:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-008</t>
-  </si>
-  <si>
-    <t>BBDD</t>
-  </si>
-  <si>
-    <t>Bases de Datos</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>GIISOF01-4-005</t>
-  </si>
-  <si>
-    <t>ASLEPI</t>
-  </si>
-  <si>
-    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática (80)</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-003</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>Estructura de Datos</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-011</t>
-  </si>
-  <si>
-    <t>IFA</t>
-  </si>
-  <si>
-    <t>Informática Forense y Auditoría</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-008</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-005</t>
-  </si>
-  <si>
-    <t>OyE</t>
-  </si>
-  <si>
-    <t>Ondas y Electromagnetismo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-013 </t>
-  </si>
-  <si>
-    <t>GIISOF01-2-004</t>
-  </si>
-  <si>
-    <t>TPP</t>
-  </si>
-  <si>
-    <t>Tecnología y Paradigmas de Programación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-009 </t>
-  </si>
-  <si>
-    <t>DLP</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
-  </si>
-  <si>
-    <t>3:30:00</t>
-  </si>
-  <si>
-    <t>18:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-004</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>Diseño del Software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-009 </t>
-  </si>
-  <si>
-    <t>20:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-016</t>
-  </si>
-  <si>
-    <t>SEV</t>
-  </si>
-  <si>
-    <t>Software de entretenimiento y videojuegos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-001 </t>
-  </si>
-  <si>
-    <t>GIISOF01-1-004</t>
-  </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Cálculo</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-007</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Introducción a la Programación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-004 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-010 </t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-006</t>
-  </si>
-  <si>
-    <t>Est</t>
-  </si>
-  <si>
-    <t>Estadística</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-006</t>
-  </si>
-  <si>
-    <t>ASR</t>
-  </si>
-  <si>
-    <t>Administración de Sistemas y Redes</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-010</t>
-  </si>
-  <si>
-    <t>IAE</t>
-  </si>
-  <si>
-    <t>Integración de aplicaciones empresariales</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-003</t>
-  </si>
-  <si>
-    <t>IPS</t>
-  </si>
-  <si>
-    <t>Ingeniería del Proceso Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-010</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>Metodología de la Programación</t>
   </si>
 </sst>
 </file>
@@ -717,7 +702,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -738,12 +723,12 @@
         <v>0.0</v>
       </c>
       <c r="P2" t="n">
-        <v>3.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B3" t="n">
         <v>1.0</v>
@@ -758,19 +743,19 @@
         <v>27</v>
       </c>
       <c r="F3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="s">
         <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
       </c>
       <c r="K3" t="n">
         <v>44361.0</v>
@@ -782,42 +767,42 @@
         <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O3" t="n">
         <v>0.0</v>
       </c>
       <c r="P3" t="n">
-        <v>42.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
@@ -829,48 +814,48 @@
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O4" t="n">
         <v>0.0</v>
       </c>
       <c r="P4" t="n">
-        <v>34.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" t="n">
         <v>1.0</v>
       </c>
       <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G5" t="s">
         <v>38</v>
       </c>
-      <c r="F5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>39</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J5" t="s">
         <v>40</v>
-      </c>
-      <c r="I5" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>41</v>
       </c>
       <c r="K5" t="n">
         <v>44361.0</v>
@@ -879,116 +864,116 @@
         <v>22</v>
       </c>
       <c r="M5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="N5" t="s">
-        <v>43</v>
-      </c>
       <c r="O5" t="n">
         <v>0.0</v>
       </c>
       <c r="P5" t="n">
-        <v>8.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
       <c r="F6" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0</v>
+        <v>90.0</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K6" t="n">
         <v>44362.0</v>
       </c>
       <c r="L6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M6" t="s">
         <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="O6" t="n">
         <v>0.0</v>
       </c>
       <c r="P6" t="n">
-        <v>48.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B7" t="n">
         <v>1.0</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F7" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="K7" t="n">
         <v>44362.0</v>
       </c>
       <c r="L7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
         <v>49</v>
       </c>
-      <c r="N7" t="s">
-        <v>53</v>
-      </c>
       <c r="O7" t="n">
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>36.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="8">
@@ -996,699 +981,699 @@
         <v>2.0</v>
       </c>
       <c r="B8" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F8" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I8" t="n">
-        <v>50.0</v>
+        <v>8.0</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K8" t="n">
         <v>44362.0</v>
       </c>
       <c r="L8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O8" t="n">
         <v>0.0</v>
       </c>
       <c r="P8" t="n">
-        <v>18.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B9" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>59</v>
-      </c>
       <c r="F9" t="n">
         <v>1.0</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I9" t="n">
-        <v>40.0</v>
+        <v>67.0</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K9" t="n">
         <v>44362.0</v>
       </c>
       <c r="L9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O9" t="n">
         <v>0.0</v>
       </c>
       <c r="P9" t="n">
-        <v>31.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B10" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="F10" t="n">
         <v>1.0</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I10" t="n">
-        <v>120.0</v>
+        <v>0.0</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K10" t="n">
         <v>44363.0</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s">
         <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O10" t="n">
         <v>0.0</v>
       </c>
       <c r="P10" t="n">
-        <v>45.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F11" t="n">
         <v>1.0</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I11" t="n">
-        <v>120.0</v>
+        <v>177.0</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K11" t="n">
         <v>44363.0</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" t="s">
         <v>66</v>
       </c>
-      <c r="N11" t="s">
-        <v>70</v>
-      </c>
       <c r="O11" t="n">
         <v>0.0</v>
       </c>
       <c r="P11" t="n">
-        <v>56.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I12" t="n">
-        <v>116.0</v>
+        <v>60.0</v>
       </c>
       <c r="J12" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="K12" t="n">
         <v>44363.0</v>
       </c>
       <c r="L12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M12" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O12" t="n">
         <v>0.0</v>
       </c>
       <c r="P12" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B13" t="n">
         <v>1.0</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F13" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="J13" t="s">
         <v>40</v>
-      </c>
-      <c r="I13" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>64</v>
       </c>
       <c r="K13" t="n">
         <v>44363.0</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M13" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="N13" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="O13" t="n">
         <v>0.0</v>
       </c>
       <c r="P13" t="n">
-        <v>28.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B14" t="n">
         <v>1.0</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="F14" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="I14" t="n">
         <v>0.0</v>
       </c>
       <c r="J14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K14" t="n">
         <v>44364.0</v>
       </c>
       <c r="L14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M14" t="s">
         <v>23</v>
       </c>
       <c r="N14" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="O14" t="n">
         <v>0.0</v>
       </c>
       <c r="P14" t="n">
-        <v>33.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
         <v>81</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>82</v>
       </c>
-      <c r="E15" t="s">
-        <v>83</v>
-      </c>
       <c r="F15" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="J15" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="K15" t="n">
         <v>44364.0</v>
       </c>
       <c r="L15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M15" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="N15" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="O15" t="n">
         <v>0.0</v>
       </c>
       <c r="P15" t="n">
-        <v>20.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B16" t="n">
         <v>1.0</v>
       </c>
       <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
         <v>84</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>85</v>
       </c>
-      <c r="E16" t="s">
-        <v>86</v>
-      </c>
       <c r="F16" t="n">
         <v>1.0</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I16" t="n">
-        <v>8.0</v>
+        <v>50.0</v>
       </c>
       <c r="J16" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="K16" t="n">
         <v>44364.0</v>
       </c>
       <c r="L16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M16" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O16" t="n">
         <v>0.0</v>
       </c>
       <c r="P16" t="n">
-        <v>57.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B17" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
         <v>89</v>
       </c>
-      <c r="D17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" t="s">
-        <v>91</v>
-      </c>
       <c r="F17" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I17" t="n">
-        <v>45.0</v>
+        <v>71.0</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="K17" t="n">
         <v>44364.0</v>
       </c>
       <c r="L17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M17" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="N17" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="O17" t="n">
         <v>0.0</v>
       </c>
       <c r="P17" t="n">
-        <v>30.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="B18" t="n">
         <v>1.0</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="F18" t="n">
         <v>1.0</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I18" t="n">
-        <v>90.0</v>
+        <v>0.0</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="K18" t="n">
         <v>44365.0</v>
       </c>
       <c r="L18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M18" t="s">
         <v>23</v>
       </c>
       <c r="N18" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="O18" t="n">
         <v>0.0</v>
       </c>
       <c r="P18" t="n">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I19" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="J19" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K19" t="n">
         <v>44365.0</v>
       </c>
       <c r="L19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M19" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N19" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="O19" t="n">
         <v>0.0</v>
       </c>
       <c r="P19" t="n">
-        <v>52.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B20" t="n">
         <v>1.0</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="F20" t="n">
         <v>1.0</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I20" t="n">
-        <v>44.0</v>
+        <v>8.0</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="K20" t="n">
         <v>44365.0</v>
       </c>
       <c r="L20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M20" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="N20" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="O20" t="n">
         <v>0.0</v>
       </c>
       <c r="P20" t="n">
-        <v>38.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B21" t="n">
         <v>2.0</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="F21" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" t="n">
+        <v>183.0</v>
+      </c>
+      <c r="J21" t="s">
         <v>40</v>
-      </c>
-      <c r="I21" t="n">
-        <v>71.0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>64</v>
       </c>
       <c r="K21" t="n">
         <v>44365.0</v>
       </c>
       <c r="L21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M21" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="N21" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="O21" t="n">
         <v>0.0</v>
       </c>
       <c r="P21" t="n">
-        <v>51.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="22">
@@ -1699,28 +1684,28 @@
         <v>1.0</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F22" t="n">
         <v>1.0</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I22" t="n">
         <v>103.0</v>
       </c>
       <c r="J22" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="K22" t="n">
         <v>44368.0</v>
@@ -1749,28 +1734,28 @@
         <v>2.0</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="F23" t="n">
         <v>1.0</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I23" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J23" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="K23" t="n">
         <v>44368.0</v>
@@ -1782,45 +1767,45 @@
         <v>66</v>
       </c>
       <c r="N23" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="O23" t="n">
         <v>0.0</v>
       </c>
       <c r="P23" t="n">
-        <v>15.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B24" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H24" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I24" t="n">
-        <v>84.0</v>
+        <v>50.0</v>
       </c>
       <c r="J24" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="K24" t="n">
         <v>44368.0</v>
@@ -1829,48 +1814,48 @@
         <v>22</v>
       </c>
       <c r="M24" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="N24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O24" t="n">
         <v>0.0</v>
       </c>
       <c r="P24" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B25" t="n">
         <v>2.0</v>
       </c>
       <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
         <v>112</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>113</v>
       </c>
-      <c r="E25" t="s">
-        <v>114</v>
-      </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G25" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="H25" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I25" t="n">
-        <v>20.0</v>
+        <v>71.0</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="K25" t="n">
         <v>44368.0</v>
@@ -1879,74 +1864,74 @@
         <v>22</v>
       </c>
       <c r="M25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N25" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="O25" t="n">
         <v>0.0</v>
       </c>
       <c r="P25" t="n">
-        <v>61.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B26" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
         <v>115</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>116</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="J26" t="s">
         <v>117</v>
-      </c>
-      <c r="F26" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>21</v>
       </c>
       <c r="K26" t="n">
         <v>44369.0</v>
       </c>
       <c r="L26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M26" t="s">
         <v>23</v>
       </c>
       <c r="N26" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="O26" t="n">
         <v>0.0</v>
       </c>
       <c r="P26" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B27" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
@@ -1961,42 +1946,42 @@
         <v>1.0</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I27" t="n">
-        <v>100.0</v>
+        <v>45.0</v>
       </c>
       <c r="J27" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="K27" t="n">
         <v>44369.0</v>
       </c>
       <c r="L27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M27" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="N27" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="O27" t="n">
         <v>0.0</v>
       </c>
       <c r="P27" t="n">
-        <v>24.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B28" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C28" t="s">
         <v>121</v>
@@ -2008,54 +1993,54 @@
         <v>123</v>
       </c>
       <c r="F28" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G28" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H28" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I28" t="n">
-        <v>70.0</v>
+        <v>3.0</v>
       </c>
       <c r="J28" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="K28" t="n">
         <v>44369.0</v>
       </c>
       <c r="L28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M28" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="N28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="O28" t="n">
         <v>0.0</v>
       </c>
       <c r="P28" t="n">
-        <v>32.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="F29" t="n">
         <v>1.0</v>
@@ -2064,501 +2049,501 @@
         <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I29" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="J29" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="K29" t="n">
         <v>44369.0</v>
       </c>
       <c r="L29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M29" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="N29" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O29" t="n">
         <v>0.0</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B30" t="n">
         <v>2.0</v>
       </c>
       <c r="C30" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F30" t="n">
         <v>2.0</v>
       </c>
       <c r="G30" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="H30" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="I30" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="J30" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="K30" t="n">
         <v>44370.0</v>
       </c>
       <c r="L30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M30" t="s">
         <v>23</v>
       </c>
       <c r="N30" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="O30" t="n">
         <v>0.0</v>
       </c>
       <c r="P30" t="n">
-        <v>22.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B31" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="E31" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="F31" t="n">
         <v>1.0</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H31" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I31" t="n">
-        <v>71.0</v>
+        <v>0.0</v>
       </c>
       <c r="J31" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K31" t="n">
         <v>44370.0</v>
       </c>
       <c r="L31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M31" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="N31" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="O31" t="n">
         <v>0.0</v>
       </c>
       <c r="P31" t="n">
-        <v>55.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B32" t="n">
         <v>2.0</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F32" t="n">
         <v>1.0</v>
       </c>
       <c r="G32" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J32" t="s">
         <v>40</v>
-      </c>
-      <c r="I32" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="J32" t="s">
-        <v>41</v>
       </c>
       <c r="K32" t="n">
         <v>44370.0</v>
       </c>
       <c r="L32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M32" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="N32" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="O32" t="n">
         <v>0.0</v>
       </c>
       <c r="P32" t="n">
-        <v>14.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="B33" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C33" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F33" t="n">
         <v>1.0</v>
       </c>
       <c r="G33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H33" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="I33" t="n">
-        <v>177.0</v>
+        <v>0.0</v>
       </c>
       <c r="J33" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="K33" t="n">
         <v>44370.0</v>
       </c>
       <c r="L33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M33" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="N33" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="O33" t="n">
         <v>0.0</v>
       </c>
       <c r="P33" t="n">
-        <v>53.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B34" t="n">
         <v>1.0</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>140</v>
+        <v>27</v>
       </c>
       <c r="F34" t="n">
         <v>2.0</v>
       </c>
       <c r="G34" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H34" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I34" t="n">
-        <v>79.0</v>
+        <v>0.0</v>
       </c>
       <c r="J34" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="K34" t="n">
         <v>44371.0</v>
       </c>
       <c r="L34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M34" t="s">
         <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="O34" t="n">
         <v>0.0</v>
       </c>
       <c r="P34" t="n">
-        <v>29.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B35" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="F35" t="n">
         <v>1.0</v>
       </c>
       <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" t="s">
+        <v>33</v>
+      </c>
+      <c r="I35" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="J35" t="s">
         <v>28</v>
-      </c>
-      <c r="H35" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" t="n">
-        <v>62.0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>30</v>
       </c>
       <c r="K35" t="n">
         <v>44371.0</v>
       </c>
       <c r="L35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M35" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="N35" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="O35" t="n">
         <v>0.0</v>
       </c>
       <c r="P35" t="n">
-        <v>35.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B36" t="n">
         <v>1.0</v>
       </c>
       <c r="C36" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F36" t="n">
         <v>1.0</v>
       </c>
       <c r="G36" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H36" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I36" t="n">
-        <v>3.0</v>
+        <v>62.0</v>
       </c>
       <c r="J36" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="K36" t="n">
         <v>44371.0</v>
       </c>
       <c r="L36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M36" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="N36" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="O36" t="n">
         <v>0.0</v>
       </c>
       <c r="P36" t="n">
-        <v>41.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B37" t="n">
         <v>2.0</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D37" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="E37" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F37" t="n">
         <v>1.0</v>
       </c>
       <c r="G37" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H37" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I37" t="n">
-        <v>0.0</v>
+        <v>150.0</v>
       </c>
       <c r="J37" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="K37" t="n">
         <v>44371.0</v>
       </c>
       <c r="L37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M37" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="N37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O37" t="n">
         <v>0.0</v>
       </c>
       <c r="P37" t="n">
-        <v>21.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B38" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E38" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F38" t="n">
         <v>1.0</v>
       </c>
       <c r="G38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H38" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I38" t="n">
-        <v>150.0</v>
+        <v>0.0</v>
       </c>
       <c r="J38" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="K38" t="n">
         <v>44372.0</v>
       </c>
       <c r="L38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M38" t="s">
         <v>23</v>
       </c>
       <c r="N38" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="O38" t="n">
         <v>0.0</v>
       </c>
       <c r="P38" t="n">
-        <v>26.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B39" t="n">
         <v>1.0</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="E39" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="F39" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G39" t="s">
         <v>19</v>
@@ -2567,7 +2552,7 @@
         <v>20</v>
       </c>
       <c r="I39" t="n">
-        <v>0.0</v>
+        <v>84.0</v>
       </c>
       <c r="J39" t="s">
         <v>21</v>
@@ -2576,151 +2561,151 @@
         <v>44372.0</v>
       </c>
       <c r="L39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M39" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N39" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="O39" t="n">
         <v>0.0</v>
       </c>
       <c r="P39" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B40" t="n">
         <v>2.0</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F40" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G40" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="H40" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I40" t="n">
-        <v>61.0</v>
+        <v>89.0</v>
       </c>
       <c r="J40" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="K40" t="n">
         <v>44372.0</v>
       </c>
       <c r="L40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M40" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="N40" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="O40" t="n">
         <v>0.0</v>
       </c>
       <c r="P40" t="n">
-        <v>7.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B41" t="n">
         <v>2.0</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E41" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F41" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H41" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I41" t="n">
-        <v>89.0</v>
+        <v>120.0</v>
       </c>
       <c r="J41" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="K41" t="n">
         <v>44372.0</v>
       </c>
       <c r="L41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N41" t="s">
-        <v>159</v>
+        <v>90</v>
       </c>
       <c r="O41" t="n">
         <v>0.0</v>
       </c>
       <c r="P41" t="n">
-        <v>58.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B42" t="n">
         <v>2.0</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="D42" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="E42" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
       </c>
       <c r="G42" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H42" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I42" t="n">
-        <v>60.0</v>
+        <v>116.0</v>
       </c>
       <c r="J42" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K42" t="n">
         <v>44375.0</v>
@@ -2732,45 +2717,45 @@
         <v>23</v>
       </c>
       <c r="N42" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="O42" t="n">
         <v>0.0</v>
       </c>
       <c r="P42" t="n">
-        <v>39.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B43" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D43" t="s">
-        <v>161</v>
+        <v>81</v>
       </c>
       <c r="E43" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="F43" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G43" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H43" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I43" t="n">
-        <v>150.0</v>
+        <v>30.0</v>
       </c>
       <c r="J43" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="K43" t="n">
         <v>44375.0</v>
@@ -2779,16 +2764,16 @@
         <v>22</v>
       </c>
       <c r="M43" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="N43" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="O43" t="n">
         <v>0.0</v>
       </c>
       <c r="P43" t="n">
-        <v>2.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="44">
@@ -2799,28 +2784,28 @@
         <v>2.0</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D44" t="s">
         <v>14</v>
       </c>
       <c r="E44" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="F44" t="n">
         <v>2.0</v>
       </c>
       <c r="G44" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="H44" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I44" t="n">
         <v>50.0</v>
       </c>
       <c r="J44" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K44" t="n">
         <v>44375.0</v>
@@ -2829,10 +2814,10 @@
         <v>22</v>
       </c>
       <c r="M44" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="N44" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="O44" t="n">
         <v>0.0</v>
@@ -2849,28 +2834,28 @@
         <v>2.0</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="D45" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="E45" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="F45" t="n">
         <v>1.0</v>
       </c>
       <c r="G45" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H45" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0</v>
+        <v>70.0</v>
       </c>
       <c r="J45" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="K45" t="n">
         <v>44375.0</v>
@@ -2879,83 +2864,83 @@
         <v>22</v>
       </c>
       <c r="M45" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="N45" t="s">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="O45" t="n">
         <v>0.0</v>
       </c>
       <c r="P45" t="n">
-        <v>23.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B46" t="n">
         <v>1.0</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>156</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>157</v>
       </c>
       <c r="E46" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
       <c r="F46" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G46" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H46" t="s">
-        <v>131</v>
+        <v>47</v>
       </c>
       <c r="I46" t="n">
         <v>0.0</v>
       </c>
       <c r="J46" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="K46" t="n">
         <v>44376.0</v>
       </c>
       <c r="L46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M46" t="s">
         <v>23</v>
       </c>
       <c r="N46" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="O46" t="n">
         <v>0.0</v>
       </c>
       <c r="P46" t="n">
-        <v>43.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B47" t="n">
         <v>1.0</v>
       </c>
       <c r="C47" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="D47" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="E47" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="F47" t="n">
         <v>1.0</v>
@@ -2964,181 +2949,181 @@
         <v>19</v>
       </c>
       <c r="H47" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0</v>
+        <v>62.0</v>
       </c>
       <c r="J47" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="K47" t="n">
         <v>44376.0</v>
       </c>
       <c r="L47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M47" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N47" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="O47" t="n">
         <v>0.0</v>
       </c>
       <c r="P47" t="n">
-        <v>54.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B48" t="n">
         <v>1.0</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D48" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="E48" t="s">
-        <v>86</v>
+        <v>161</v>
       </c>
       <c r="F48" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G48" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H48" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I48" t="n">
-        <v>8.0</v>
+        <v>140.0</v>
       </c>
       <c r="J48" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="K48" t="n">
         <v>44376.0</v>
       </c>
       <c r="L48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M48" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="N48" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="O48" t="n">
         <v>0.0</v>
       </c>
       <c r="P48" t="n">
-        <v>59.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B49" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="E49" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="F49" t="n">
         <v>1.0</v>
       </c>
       <c r="G49" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H49" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I49" t="n">
-        <v>67.0</v>
+        <v>61.0</v>
       </c>
       <c r="J49" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="K49" t="n">
         <v>44377.0</v>
       </c>
       <c r="L49" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M49" t="s">
         <v>23</v>
       </c>
       <c r="N49" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="O49" t="n">
         <v>0.0</v>
       </c>
       <c r="P49" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B50" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="D50" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E50" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="F50" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G50" t="s">
+        <v>38</v>
+      </c>
+      <c r="H50" t="s">
         <v>39</v>
       </c>
-      <c r="H50" t="s">
-        <v>40</v>
-      </c>
       <c r="I50" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="J50" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="K50" t="n">
         <v>44377.0</v>
       </c>
       <c r="L50" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M50" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="N50" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="O50" t="n">
         <v>0.0</v>
       </c>
       <c r="P50" t="n">
-        <v>4.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="51">
@@ -3146,149 +3131,149 @@
         <v>1.0</v>
       </c>
       <c r="B51" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C51" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="D51" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E51" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F51" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G51" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H51" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I51" t="n">
-        <v>140.0</v>
+        <v>70.0</v>
       </c>
       <c r="J51" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K51" t="n">
         <v>44377.0</v>
       </c>
       <c r="L51" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M51" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="N51" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="O51" t="n">
         <v>0.0</v>
       </c>
       <c r="P51" t="n">
-        <v>40.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B52" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C52" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="D52" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
       <c r="E52" t="s">
-        <v>59</v>
+        <v>169</v>
       </c>
       <c r="F52" t="n">
         <v>1.0</v>
       </c>
       <c r="G52" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H52" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I52" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="J52" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="K52" t="n">
         <v>44378.0</v>
       </c>
       <c r="L52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M52" t="s">
         <v>23</v>
       </c>
       <c r="N52" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="O52" t="n">
         <v>0.0</v>
       </c>
       <c r="P52" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B53" t="n">
         <v>1.0</v>
       </c>
       <c r="C53" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D53" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="E53" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="F53" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G53" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="H53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J53" t="s">
         <v>40</v>
-      </c>
-      <c r="I53" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="J53" t="s">
-        <v>64</v>
       </c>
       <c r="K53" t="n">
         <v>44378.0</v>
       </c>
       <c r="L53" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M53" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="N53" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="O53" t="n">
         <v>0.0</v>
       </c>
       <c r="P53" t="n">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="54">
@@ -3299,196 +3284,196 @@
         <v>1.0</v>
       </c>
       <c r="C54" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D54" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E54" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F54" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G54" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H54" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I54" t="n">
-        <v>79.0</v>
+        <v>150.0</v>
       </c>
       <c r="J54" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="K54" t="n">
         <v>44378.0</v>
       </c>
       <c r="L54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M54" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="N54" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="O54" t="n">
         <v>0.0</v>
       </c>
       <c r="P54" t="n">
-        <v>37.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C55" t="s">
+        <v>174</v>
+      </c>
+      <c r="D55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" t="s">
         <v>176</v>
       </c>
-      <c r="D55" t="s">
-        <v>119</v>
-      </c>
-      <c r="E55" t="s">
-        <v>120</v>
-      </c>
       <c r="F55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G55" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H55" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I55" t="n">
-        <v>30.0</v>
+        <v>44.0</v>
       </c>
       <c r="J55" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="K55" t="n">
         <v>44379.0</v>
       </c>
       <c r="L55" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M55" t="s">
         <v>23</v>
       </c>
       <c r="N55" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="O55" t="n">
         <v>0.0</v>
       </c>
       <c r="P55" t="n">
-        <v>46.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B56" t="n">
         <v>2.0</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="D56" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="E56" t="s">
-        <v>177</v>
+        <v>113</v>
       </c>
       <c r="F56" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G56" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H56" t="s">
+        <v>33</v>
+      </c>
+      <c r="I56" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="J56" t="s">
         <v>40</v>
-      </c>
-      <c r="I56" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="J56" t="s">
-        <v>158</v>
       </c>
       <c r="K56" t="n">
         <v>44379.0</v>
       </c>
       <c r="L56" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M56" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="N56" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="O56" t="n">
         <v>0.0</v>
       </c>
       <c r="P56" t="n">
-        <v>60.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B57" t="n">
         <v>2.0</v>
       </c>
       <c r="C57" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" t="s">
         <v>178</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>179</v>
       </c>
-      <c r="E57" t="s">
-        <v>180</v>
-      </c>
       <c r="F57" t="n">
         <v>1.0</v>
       </c>
       <c r="G57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H57" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I57" t="n">
-        <v>183.0</v>
+        <v>0.0</v>
       </c>
       <c r="J57" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="K57" t="n">
         <v>44379.0</v>
       </c>
       <c r="L57" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N57" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="O57" t="n">
         <v>0.0</v>
       </c>
       <c r="P57" t="n">
-        <v>47.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="58">
@@ -3496,16 +3481,16 @@
         <v>3.0</v>
       </c>
       <c r="B58" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C58" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" t="s">
         <v>181</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>182</v>
-      </c>
-      <c r="E58" t="s">
-        <v>183</v>
       </c>
       <c r="F58" t="n">
         <v>1.0</v>
@@ -3514,10 +3499,10 @@
         <v>19</v>
       </c>
       <c r="H58" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I58" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="J58" t="s">
         <v>21</v>
@@ -3538,39 +3523,39 @@
         <v>0.0</v>
       </c>
       <c r="P58" t="n">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B59" t="n">
         <v>1.0</v>
       </c>
       <c r="C59" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
+        <v>168</v>
       </c>
       <c r="E59" t="s">
-        <v>83</v>
+        <v>183</v>
       </c>
       <c r="F59" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G59" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H59" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I59" t="n">
-        <v>0.0</v>
+        <v>79.0</v>
       </c>
       <c r="J59" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="K59" t="n">
         <v>44382.0</v>
@@ -3582,45 +3567,45 @@
         <v>24</v>
       </c>
       <c r="N59" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="O59" t="n">
         <v>0.0</v>
       </c>
       <c r="P59" t="n">
-        <v>19.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B60" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C60" t="s">
-        <v>184</v>
+        <v>30</v>
       </c>
       <c r="D60" t="s">
-        <v>185</v>
+        <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>186</v>
+        <v>32</v>
       </c>
       <c r="F60" t="n">
         <v>1.0</v>
       </c>
       <c r="G60" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H60" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I60" t="n">
-        <v>3.0</v>
+        <v>40.0</v>
       </c>
       <c r="J60" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="K60" t="n">
         <v>44382.0</v>
@@ -3629,16 +3614,16 @@
         <v>22</v>
       </c>
       <c r="M60" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="N60" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="O60" t="n">
         <v>0.0</v>
       </c>
       <c r="P60" t="n">
-        <v>25.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="61">
@@ -3649,146 +3634,146 @@
         <v>1.0</v>
       </c>
       <c r="C61" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D61" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="E61" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="F61" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G61" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H61" t="s">
+        <v>33</v>
+      </c>
+      <c r="I61" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="J61" t="s">
         <v>40</v>
-      </c>
-      <c r="I61" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="J61" t="s">
-        <v>87</v>
       </c>
       <c r="K61" t="n">
         <v>44383.0</v>
       </c>
       <c r="L61" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M61" t="s">
         <v>23</v>
       </c>
       <c r="N61" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="O61" t="n">
         <v>0.0</v>
       </c>
       <c r="P61" t="n">
-        <v>11.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B62" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C62" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D62" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E62" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F62" t="n">
         <v>1.0</v>
       </c>
       <c r="G62" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H62" t="s">
+        <v>33</v>
+      </c>
+      <c r="I62" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="J62" t="s">
         <v>40</v>
-      </c>
-      <c r="I62" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="J62" t="s">
-        <v>30</v>
       </c>
       <c r="K62" t="n">
         <v>44383.0</v>
       </c>
       <c r="L62" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M62" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="N62" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="O62" t="n">
         <v>0.0</v>
       </c>
       <c r="P62" t="n">
-        <v>17.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B63" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C63" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D63" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E63" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="F63" t="n">
         <v>1.0</v>
       </c>
       <c r="G63" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H63" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I63" t="n">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="J63" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="K63" t="n">
         <v>44383.0</v>
       </c>
       <c r="L63" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N63" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="O63" t="n">
         <v>0.0</v>
       </c>
       <c r="P63" t="n">
-        <v>12.0</v>
+        <v>23.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Half of the project documented with Javadoc
</commit_message>
<xml_diff>
--- a/files/output/prueba.xlsx
+++ b/files/output/prueba.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="193">
   <si>
     <t>Curso</t>
   </si>
@@ -62,6 +62,171 @@
     <t>ID</t>
   </si>
   <si>
+    <t>GIISOF01-0-013</t>
+  </si>
+  <si>
+    <t>SDM</t>
+  </si>
+  <si>
+    <t>Software para Dispositivos Móviles</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>0:30:00</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>9:00:00</t>
+  </si>
+  <si>
+    <t>9:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-010 </t>
+  </si>
+  <si>
+    <t>Alg</t>
+  </si>
+  <si>
+    <t>Algoritmia</t>
+  </si>
+  <si>
+    <t>Práctico</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>2:00:00</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-002 </t>
+  </si>
+  <si>
+    <t>SEW</t>
+  </si>
+  <si>
+    <t>Software y Estándares para la Web</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-006</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Estadística</t>
+  </si>
+  <si>
+    <t>Teórico</t>
+  </si>
+  <si>
+    <t>3:00:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-002</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Álgebra Lineal</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-001</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Repositorios de Información</t>
+  </si>
+  <si>
+    <t>12:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-006</t>
+  </si>
+  <si>
+    <t>SSOO</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos</t>
+  </si>
+  <si>
+    <t>1:00:00</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-008</t>
+  </si>
+  <si>
+    <t>BBDD</t>
+  </si>
+  <si>
+    <t>Bases de Datos</t>
+  </si>
+  <si>
+    <t>2:30:00</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t>miércoles</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-009</t>
+  </si>
+  <si>
+    <t>Computación Numérica</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-004</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Diseño del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-004</t>
+  </si>
+  <si>
+    <t>DPPI</t>
+  </si>
+  <si>
+    <t>Dirección y Planificación de Proyectos Informáticos</t>
+  </si>
+  <si>
+    <t>No presencial</t>
+  </si>
+  <si>
+    <t>20:00:00</t>
+  </si>
+  <si>
     <t>GIISOF01-0-010</t>
   </si>
   <si>
@@ -71,19 +236,7 @@
     <t>Integración de aplicaciones empresariales</t>
   </si>
   <si>
-    <t>Teórico</t>
-  </si>
-  <si>
-    <t>No presencial</t>
-  </si>
-  <si>
-    <t>1:00:00</t>
-  </si>
-  <si>
-    <t>lunes</t>
-  </si>
-  <si>
-    <t>9:00:00</t>
+    <t>jueves</t>
   </si>
   <si>
     <t>10:00:00</t>
@@ -98,484 +251,346 @@
     <t>Sistemas de Información para la Web</t>
   </si>
   <si>
-    <t>2:00:00</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-006</t>
-  </si>
-  <si>
-    <t>SSOO</t>
-  </si>
-  <si>
-    <t>Sistemas Operativos</t>
-  </si>
-  <si>
-    <t>Presencial</t>
+    <t xml:space="preserve">GIISOF01-3-004 </t>
+  </si>
+  <si>
+    <t>GIISOF01-2-002</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Arquitectura de Computadores</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-003</t>
+  </si>
+  <si>
+    <t>CVVS</t>
+  </si>
+  <si>
+    <t>Calidad, Validación y Verificación del Software</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-009</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>GIISOF01-2-001</t>
+  </si>
+  <si>
+    <t>TEC</t>
+  </si>
+  <si>
+    <t>Tecnología Electrónica de Computadores</t>
   </si>
   <si>
     <t>13:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">GIISOF01-3-002 </t>
-  </si>
-  <si>
-    <t>SEW</t>
-  </si>
-  <si>
-    <t>Software y Estándares para la Web</t>
-  </si>
-  <si>
-    <t>Trabajo</t>
+    <t>GIISOF01-3-003</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>Ingeniería del Proceso Software</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-005</t>
+  </si>
+  <si>
+    <t>ASLEPI</t>
+  </si>
+  <si>
+    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-003</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Estructura de Datos</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-007</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Introducción a la Programación</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-008 </t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Arquitectura del Software</t>
   </si>
   <si>
     <t>Presentación</t>
   </si>
   <si>
-    <t>3:00:00</t>
-  </si>
-  <si>
-    <t>15:00:00</t>
+    <t xml:space="preserve">GIISOF01-3-009 </t>
+  </si>
+  <si>
+    <t>DLP</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
+  </si>
+  <si>
+    <t>3:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-009 </t>
+  </si>
+  <si>
+    <t>15:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-016</t>
+  </si>
+  <si>
+    <t>SEV</t>
+  </si>
+  <si>
+    <t>Software de entretenimiento y videojuegos</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-010</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Metodología de la Programación</t>
+  </si>
+  <si>
+    <t>19:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-008</t>
+  </si>
+  <si>
+    <t>FCR</t>
+  </si>
+  <si>
+    <t>Fundamentos de Computadores y Redes</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-005</t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>Sistemas Distribuidos e Internet</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-017</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Software para Robots</t>
+  </si>
+  <si>
+    <t>Autómatas y Matemáticas Discretas</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-001 </t>
+  </si>
+  <si>
+    <t>GIISOF01-3-002</t>
+  </si>
+  <si>
+    <t>1:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-011</t>
+  </si>
+  <si>
+    <t>IFA</t>
+  </si>
+  <si>
+    <t>Informática Forense y Auditoría</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-010 </t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Seguridad de Sistemas Informáticos</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-002</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Ingeniería de Requisitos</t>
   </si>
   <si>
     <t>18:00:00</t>
   </si>
   <si>
-    <t>GIISOF01-4-002</t>
-  </si>
-  <si>
-    <t>IR</t>
-  </si>
-  <si>
-    <t>Ingeniería de Requisitos</t>
-  </si>
-  <si>
-    <t>martes</t>
-  </si>
-  <si>
-    <t>Entrega</t>
-  </si>
-  <si>
-    <t>0:30:00</t>
-  </si>
-  <si>
-    <t>12:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-001 </t>
-  </si>
-  <si>
-    <t>TEC</t>
-  </si>
-  <si>
-    <t>Tecnología Electrónica de Computadores</t>
-  </si>
-  <si>
-    <t>Práctico</t>
-  </si>
-  <si>
-    <t>13:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-001</t>
-  </si>
-  <si>
-    <t>RI</t>
-  </si>
-  <si>
-    <t>Repositorios de Información</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-002</t>
-  </si>
-  <si>
-    <t>1:30:00</t>
-  </si>
-  <si>
-    <t>miércoles</t>
+    <t>GIISOF01-1-003</t>
+  </si>
+  <si>
+    <t>Emp</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>20:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-008</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-005</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>Computabilidad</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-005</t>
+  </si>
+  <si>
+    <t>OyE</t>
+  </si>
+  <si>
+    <t>Ondas y Electromagnetismo</t>
+  </si>
+  <si>
+    <t>18:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-0-013 </t>
+  </si>
+  <si>
+    <t>GIISOF01-2-007</t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>Comunicación Persona-Máquina</t>
   </si>
   <si>
     <t>10:30:00</t>
   </si>
   <si>
-    <t>GIISOF01-4-005</t>
-  </si>
-  <si>
-    <t>ASLEPI</t>
-  </si>
-  <si>
-    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-002</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Arquitectura de Computadores</t>
-  </si>
-  <si>
-    <t>2:30:00</t>
+    <t xml:space="preserve">GIISOF01-2-007 </t>
+  </si>
+  <si>
+    <t>GIISOF01-1-004</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Cálculo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-005 </t>
+  </si>
+  <si>
+    <t>16:30:00</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-008</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Sistemas Inteligentes</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-006</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Administración de Sistemas y Redes</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-004</t>
+  </si>
+  <si>
+    <t>TPP</t>
+  </si>
+  <si>
+    <t>Tecnología y Paradigmas de Programación</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-001</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática (80)</t>
   </si>
   <si>
     <t>14:00:00</t>
   </si>
   <si>
-    <t>GIISOF01-1-002</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>Álgebra Lineal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-013 </t>
-  </si>
-  <si>
-    <t>SDM</t>
-  </si>
-  <si>
-    <t>Software para Dispositivos Móviles</t>
-  </si>
-  <si>
-    <t>jueves</t>
-  </si>
-  <si>
-    <t>9:30:00</t>
+    <t>GIISOF01-0-018</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Informática Audiovisual</t>
   </si>
   <si>
     <t>GIISOF01-2-010</t>
   </si>
   <si>
-    <t>Alg</t>
-  </si>
-  <si>
-    <t>Algoritmia</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-007</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Introducción a la Programación</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-010 </t>
-  </si>
-  <si>
-    <t>SSI</t>
-  </si>
-  <si>
-    <t>Seguridad de Sistemas Informáticos</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-013</t>
-  </si>
-  <si>
-    <t>viernes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-005 </t>
-  </si>
-  <si>
-    <t>SDI</t>
-  </si>
-  <si>
-    <t>Sistemas Distribuidos e Internet</t>
-  </si>
-  <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-001</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-006</t>
-  </si>
-  <si>
-    <t>Est</t>
-  </si>
-  <si>
-    <t>Estadística</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-008</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Sistemas Inteligentes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-008</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-010</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>Metodología de la Programación</t>
-  </si>
-  <si>
-    <t>15:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-008</t>
-  </si>
-  <si>
-    <t>BBDD</t>
-  </si>
-  <si>
-    <t>Bases de Datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-009 </t>
-  </si>
-  <si>
-    <t>DLP</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
-  </si>
-  <si>
-    <t>3:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-003</t>
-  </si>
-  <si>
-    <t>CVVS</t>
-  </si>
-  <si>
-    <t>Calidad, Validación y Verificación del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-011</t>
-  </si>
-  <si>
-    <t>IFA</t>
-  </si>
-  <si>
-    <t>Informática Forense y Auditoría</t>
-  </si>
-  <si>
-    <t>18:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-008</t>
-  </si>
-  <si>
-    <t>FCR</t>
-  </si>
-  <si>
-    <t>Fundamentos de Computadores y Redes</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-009</t>
-  </si>
-  <si>
-    <t>Computación Numérica</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-017</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>Software para Robots</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-005</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-003</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>Estructura de Datos</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-005</t>
-  </si>
-  <si>
-    <t>OyE</t>
-  </si>
-  <si>
-    <t>Ondas y Electromagnetismo</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-018</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>Informática Audiovisual</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-007</t>
-  </si>
-  <si>
-    <t>CPM</t>
-  </si>
-  <si>
-    <t>Comunicación Persona-Máquina</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-004</t>
-  </si>
-  <si>
-    <t>DPPI</t>
-  </si>
-  <si>
-    <t>Dirección y Planificación de Proyectos Informáticos</t>
-  </si>
-  <si>
     <t>GIISOF01-3-010</t>
   </si>
   <si>
-    <t xml:space="preserve">GIISOF01-2-010 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-009 </t>
-  </si>
-  <si>
-    <t>GIISOF01-1-009</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>GIISOF01-0-016</t>
-  </si>
-  <si>
-    <t>SEV</t>
-  </si>
-  <si>
-    <t>Software de entretenimiento y videojuegos</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-004</t>
-  </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Cálculo</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-004</t>
-  </si>
-  <si>
-    <t>TPP</t>
-  </si>
-  <si>
-    <t>Tecnología y Paradigmas de Programación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-008 </t>
-  </si>
-  <si>
-    <t>Autómatas y Matemáticas Discretas</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-001</t>
-  </si>
-  <si>
-    <t>FI</t>
-  </si>
-  <si>
     <t>Fundamentos de Informática</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-007 </t>
-  </si>
-  <si>
-    <t>GIISOF01-3-004</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>Diseño del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-003</t>
-  </si>
-  <si>
-    <t>Emp</t>
-  </si>
-  <si>
-    <t>Empresa</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-006</t>
-  </si>
-  <si>
-    <t>ASR</t>
-  </si>
-  <si>
-    <t>Administración de Sistemas y Redes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-003</t>
-  </si>
-  <si>
-    <t>IPS</t>
-  </si>
-  <si>
-    <t>Ingeniería del Proceso Software</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática (80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-004 </t>
-  </si>
-  <si>
-    <t>GIISOF01-2-005</t>
-  </si>
-  <si>
-    <t>Comp</t>
-  </si>
-  <si>
-    <t>Computabilidad</t>
   </si>
 </sst>
 </file>
@@ -702,7 +717,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -723,15 +738,15 @@
         <v>0.0</v>
       </c>
       <c r="P2" t="n">
-        <v>25.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -743,19 +758,19 @@
         <v>27</v>
       </c>
       <c r="F3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K3" t="n">
         <v>44361.0</v>
@@ -767,42 +782,42 @@
         <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O3" t="n">
         <v>0.0</v>
       </c>
       <c r="P3" t="n">
-        <v>19.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I4" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
@@ -814,45 +829,45 @@
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O4" t="n">
         <v>0.0</v>
       </c>
       <c r="P4" t="n">
-        <v>1.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0</v>
+        <v>183.0</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
@@ -864,45 +879,45 @@
         <v>22</v>
       </c>
       <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
         <v>41</v>
       </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
       <c r="O5" t="n">
         <v>0.0</v>
       </c>
       <c r="P5" t="n">
-        <v>43.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
       </c>
       <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
       <c r="F6" t="n">
         <v>1.0</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I6" t="n">
-        <v>90.0</v>
+        <v>120.0</v>
       </c>
       <c r="J6" t="s">
         <v>40</v>
@@ -911,19 +926,19 @@
         <v>44362.0</v>
       </c>
       <c r="L6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M6" t="s">
         <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O6" t="n">
         <v>0.0</v>
       </c>
       <c r="P6" t="n">
-        <v>10.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="7">
@@ -931,40 +946,40 @@
         <v>3.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="K7" t="n">
         <v>44362.0</v>
       </c>
       <c r="L7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="N7" t="s">
         <v>49</v>
@@ -973,7 +988,7 @@
         <v>0.0</v>
       </c>
       <c r="P7" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -981,7 +996,7 @@
         <v>2.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
@@ -993,25 +1008,25 @@
         <v>52</v>
       </c>
       <c r="F8" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="J8" t="s">
         <v>53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
       </c>
       <c r="K8" t="n">
         <v>44362.0</v>
       </c>
       <c r="L8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M8" t="s">
         <v>49</v>
@@ -1023,15 +1038,15 @@
         <v>0.0</v>
       </c>
       <c r="P8" t="n">
-        <v>59.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C9" t="s">
         <v>55</v>
@@ -1046,234 +1061,234 @@
         <v>1.0</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I9" t="n">
-        <v>67.0</v>
+        <v>71.0</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="K9" t="n">
         <v>44362.0</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M9" t="s">
         <v>41</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O9" t="n">
         <v>0.0</v>
       </c>
       <c r="P9" t="n">
-        <v>9.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F10" t="n">
         <v>1.0</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K10" t="n">
         <v>44363.0</v>
       </c>
       <c r="L10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M10" t="s">
         <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="O10" t="n">
         <v>0.0</v>
       </c>
       <c r="P10" t="n">
-        <v>33.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B11" t="n">
         <v>2.0</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F11" t="n">
         <v>1.0</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I11" t="n">
-        <v>177.0</v>
+        <v>50.0</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="K11" t="n">
         <v>44363.0</v>
       </c>
       <c r="L11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M11" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="N11" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="O11" t="n">
         <v>0.0</v>
       </c>
       <c r="P11" t="n">
-        <v>53.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B12" t="n">
         <v>1.0</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F12" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I12" t="n">
-        <v>60.0</v>
+        <v>150.0</v>
       </c>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="K12" t="n">
         <v>44363.0</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="N12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="O12" t="n">
         <v>0.0</v>
       </c>
       <c r="P12" t="n">
-        <v>28.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F13" t="n">
         <v>1.0</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I13" t="n">
         <v>120.0</v>
       </c>
       <c r="J13" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K13" t="n">
         <v>44363.0</v>
       </c>
       <c r="L13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M13" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="O13" t="n">
         <v>0.0</v>
       </c>
       <c r="P13" t="n">
-        <v>56.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="14">
@@ -1284,296 +1299,296 @@
         <v>1.0</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F14" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K14" t="n">
         <v>44364.0</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M14" t="s">
         <v>23</v>
       </c>
       <c r="N14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="O14" t="n">
         <v>0.0</v>
       </c>
       <c r="P14" t="n">
-        <v>13.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B15" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F15" t="n">
         <v>1.0</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I15" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="J15" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="K15" t="n">
         <v>44364.0</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N15" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O15" t="n">
         <v>0.0</v>
       </c>
       <c r="P15" t="n">
-        <v>24.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B16" t="n">
         <v>1.0</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I16" t="n">
-        <v>50.0</v>
+        <v>79.0</v>
       </c>
       <c r="J16" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="K16" t="n">
         <v>44364.0</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M16" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="N16" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="O16" t="n">
         <v>0.0</v>
       </c>
       <c r="P16" t="n">
-        <v>44.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B17" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F17" t="n">
         <v>2.0</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I17" t="n">
-        <v>71.0</v>
+        <v>60.0</v>
       </c>
       <c r="J17" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="K17" t="n">
         <v>44364.0</v>
       </c>
       <c r="L17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M17" t="s">
         <v>41</v>
       </c>
       <c r="N17" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="O17" t="n">
         <v>0.0</v>
       </c>
       <c r="P17" t="n">
-        <v>51.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="B18" t="n">
         <v>1.0</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F18" t="n">
         <v>1.0</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="J18" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K18" t="n">
         <v>44365.0</v>
       </c>
       <c r="L18" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M18" t="s">
         <v>23</v>
       </c>
       <c r="N18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="O18" t="n">
         <v>0.0</v>
       </c>
       <c r="P18" t="n">
-        <v>3.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B19" t="n">
         <v>2.0</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F19" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G19" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H19" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0</v>
+        <v>70.0</v>
       </c>
       <c r="J19" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K19" t="n">
         <v>44365.0</v>
       </c>
       <c r="L19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N19" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="O19" t="n">
         <v>0.0</v>
       </c>
       <c r="P19" t="n">
-        <v>48.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="20">
@@ -1584,40 +1599,40 @@
         <v>1.0</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="F20" t="n">
         <v>1.0</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="I20" t="n">
         <v>8.0</v>
       </c>
       <c r="J20" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="K20" t="n">
         <v>44365.0</v>
       </c>
       <c r="L20" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M20" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="N20" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="O20" t="n">
         <v>0.0</v>
@@ -1628,52 +1643,52 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B21" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F21" t="n">
         <v>1.0</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I21" t="n">
-        <v>183.0</v>
+        <v>40.0</v>
       </c>
       <c r="J21" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="K21" t="n">
         <v>44365.0</v>
       </c>
       <c r="L21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M21" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N21" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="O21" t="n">
         <v>0.0</v>
       </c>
       <c r="P21" t="n">
-        <v>47.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="22">
@@ -1681,31 +1696,31 @@
         <v>4.0</v>
       </c>
       <c r="B22" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F22" t="n">
         <v>1.0</v>
       </c>
       <c r="G22" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I22" t="n">
-        <v>103.0</v>
+        <v>177.0</v>
       </c>
       <c r="J22" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="K22" t="n">
         <v>44368.0</v>
@@ -1717,45 +1732,45 @@
         <v>23</v>
       </c>
       <c r="N22" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="O22" t="n">
         <v>0.0</v>
       </c>
       <c r="P22" t="n">
-        <v>6.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B23" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F23" t="n">
         <v>1.0</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0</v>
+        <v>62.0</v>
       </c>
       <c r="J23" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K23" t="n">
         <v>44368.0</v>
@@ -1764,16 +1779,16 @@
         <v>22</v>
       </c>
       <c r="M23" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="N23" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="O23" t="n">
         <v>0.0</v>
       </c>
       <c r="P23" t="n">
-        <v>21.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="24">
@@ -1781,31 +1796,31 @@
         <v>1.0</v>
       </c>
       <c r="B24" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
       </c>
       <c r="G24" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I24" t="n">
         <v>50.0</v>
       </c>
       <c r="J24" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K24" t="n">
         <v>44368.0</v>
@@ -1814,48 +1829,48 @@
         <v>22</v>
       </c>
       <c r="M24" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="N24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="O24" t="n">
         <v>0.0</v>
       </c>
       <c r="P24" t="n">
-        <v>17.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B25" t="n">
         <v>2.0</v>
       </c>
       <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="I25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J25" t="s">
         <v>53</v>
-      </c>
-      <c r="H25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" t="n">
-        <v>71.0</v>
-      </c>
-      <c r="J25" t="s">
-        <v>70</v>
       </c>
       <c r="K25" t="n">
         <v>44368.0</v>
@@ -1864,16 +1879,16 @@
         <v>22</v>
       </c>
       <c r="M25" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="N25" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="O25" t="n">
         <v>0.0</v>
       </c>
       <c r="P25" t="n">
-        <v>55.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="26">
@@ -1884,34 +1899,34 @@
         <v>2.0</v>
       </c>
       <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" t="s">
         <v>114</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="J26" t="s">
         <v>115</v>
-      </c>
-      <c r="E26" t="s">
-        <v>116</v>
-      </c>
-      <c r="F26" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I26" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>117</v>
       </c>
       <c r="K26" t="n">
         <v>44369.0</v>
       </c>
       <c r="L26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M26" t="s">
         <v>23</v>
@@ -1923,57 +1938,57 @@
         <v>0.0</v>
       </c>
       <c r="P26" t="n">
-        <v>60.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="F27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G27" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I27" t="n">
-        <v>45.0</v>
+        <v>50.0</v>
       </c>
       <c r="J27" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="K27" t="n">
         <v>44369.0</v>
       </c>
       <c r="L27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M27" t="s">
         <v>49</v>
       </c>
       <c r="N27" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="O27" t="n">
         <v>0.0</v>
       </c>
       <c r="P27" t="n">
-        <v>30.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="28">
@@ -1984,13 +1999,13 @@
         <v>1.0</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F28" t="n">
         <v>1.0</v>
@@ -2002,7 +2017,7 @@
         <v>20</v>
       </c>
       <c r="I28" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="J28" t="s">
         <v>21</v>
@@ -2011,60 +2026,60 @@
         <v>44369.0</v>
       </c>
       <c r="L28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M28" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="N28" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="O28" t="n">
         <v>0.0</v>
       </c>
       <c r="P28" t="n">
-        <v>41.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B29" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="F29" t="n">
         <v>1.0</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I29" t="n">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c r="J29" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="K29" t="n">
         <v>44369.0</v>
       </c>
       <c r="L29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M29" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="N29" t="s">
         <v>124</v>
@@ -2073,7 +2088,7 @@
         <v>0.0</v>
       </c>
       <c r="P29" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="30">
@@ -2096,10 +2111,10 @@
         <v>2.0</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I30" t="n">
         <v>20.0</v>
@@ -2111,13 +2126,13 @@
         <v>44370.0</v>
       </c>
       <c r="L30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M30" t="s">
         <v>23</v>
       </c>
       <c r="N30" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O30" t="n">
         <v>0.0</v>
@@ -2128,57 +2143,57 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="F31" t="n">
         <v>1.0</v>
       </c>
       <c r="G31" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0</v>
+        <v>62.0</v>
       </c>
       <c r="J31" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K31" t="n">
         <v>44370.0</v>
       </c>
       <c r="L31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M31" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="N31" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="O31" t="n">
         <v>0.0</v>
       </c>
       <c r="P31" t="n">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B32" t="n">
         <v>2.0</v>
@@ -2187,43 +2202,43 @@
         <v>128</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F32" t="n">
         <v>1.0</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I32" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="J32" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="K32" t="n">
         <v>44370.0</v>
       </c>
       <c r="L32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M32" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="N32" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="O32" t="n">
         <v>0.0</v>
       </c>
       <c r="P32" t="n">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="33">
@@ -2234,40 +2249,40 @@
         <v>1.0</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F33" t="n">
         <v>1.0</v>
       </c>
       <c r="G33" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="H33" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I33" t="n">
         <v>0.0</v>
       </c>
       <c r="J33" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="K33" t="n">
         <v>44370.0</v>
       </c>
       <c r="L33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M33" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="N33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O33" t="n">
         <v>0.0</v>
@@ -2278,260 +2293,260 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B34" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="F34" t="n">
         <v>2.0</v>
       </c>
       <c r="G34" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H34" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0</v>
+        <v>70.0</v>
       </c>
       <c r="J34" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="K34" t="n">
         <v>44371.0</v>
       </c>
       <c r="L34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M34" t="s">
         <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="O34" t="n">
         <v>0.0</v>
       </c>
       <c r="P34" t="n">
-        <v>20.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B35" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C35" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F35" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G35" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H35" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I35" t="n">
-        <v>40.0</v>
+        <v>8.0</v>
       </c>
       <c r="J35" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="K35" t="n">
         <v>44371.0</v>
       </c>
       <c r="L35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M35" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="N35" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="O35" t="n">
         <v>0.0</v>
       </c>
       <c r="P35" t="n">
-        <v>15.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B36" t="n">
         <v>1.0</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>136</v>
+        <v>34</v>
       </c>
       <c r="F36" t="n">
         <v>1.0</v>
       </c>
       <c r="G36" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H36" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I36" t="n">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="J36" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="K36" t="n">
         <v>44371.0</v>
       </c>
       <c r="L36" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M36" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="N36" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="O36" t="n">
         <v>0.0</v>
       </c>
       <c r="P36" t="n">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B37" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F37" t="n">
         <v>1.0</v>
       </c>
       <c r="G37" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H37" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I37" t="n">
-        <v>150.0</v>
+        <v>3.0</v>
       </c>
       <c r="J37" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="K37" t="n">
         <v>44371.0</v>
       </c>
       <c r="L37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M37" t="s">
         <v>41</v>
       </c>
       <c r="N37" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="O37" t="n">
         <v>0.0</v>
       </c>
       <c r="P37" t="n">
-        <v>26.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B38" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>56</v>
       </c>
       <c r="E38" t="s">
-        <v>142</v>
+        <v>57</v>
       </c>
       <c r="F38" t="n">
         <v>1.0</v>
       </c>
       <c r="G38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H38" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="J38" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K38" t="n">
         <v>44372.0</v>
       </c>
       <c r="L38" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M38" t="s">
         <v>23</v>
       </c>
       <c r="N38" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="O38" t="n">
         <v>0.0</v>
       </c>
       <c r="P38" t="n">
-        <v>36.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B39" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C39" t="s">
         <v>143</v>
@@ -2543,137 +2558,137 @@
         <v>145</v>
       </c>
       <c r="F39" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G39" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I39" t="n">
-        <v>84.0</v>
+        <v>71.0</v>
       </c>
       <c r="J39" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="K39" t="n">
         <v>44372.0</v>
       </c>
       <c r="L39" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M39" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="N39" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="O39" t="n">
         <v>0.0</v>
       </c>
       <c r="P39" t="n">
-        <v>16.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B40" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="D40" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F40" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G40" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H40" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I40" t="n">
-        <v>89.0</v>
+        <v>90.0</v>
       </c>
       <c r="J40" t="s">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="K40" t="n">
         <v>44372.0</v>
       </c>
       <c r="L40" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M40" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="N40" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="O40" t="n">
         <v>0.0</v>
       </c>
       <c r="P40" t="n">
-        <v>58.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="B41" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E41" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F41" t="n">
         <v>1.0</v>
       </c>
       <c r="G41" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I41" t="n">
-        <v>120.0</v>
+        <v>44.0</v>
       </c>
       <c r="J41" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="K41" t="n">
         <v>44372.0</v>
       </c>
       <c r="L41" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M41" t="s">
-        <v>41</v>
+        <v>149</v>
       </c>
       <c r="N41" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="O41" t="n">
         <v>0.0</v>
       </c>
       <c r="P41" t="n">
-        <v>45.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="42">
@@ -2684,28 +2699,28 @@
         <v>2.0</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
       </c>
       <c r="G42" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H42" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I42" t="n">
-        <v>116.0</v>
+        <v>0.0</v>
       </c>
       <c r="J42" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K42" t="n">
         <v>44375.0</v>
@@ -2717,13 +2732,13 @@
         <v>23</v>
       </c>
       <c r="N42" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="O42" t="n">
         <v>0.0</v>
       </c>
       <c r="P42" t="n">
-        <v>27.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="43">
@@ -2731,31 +2746,31 @@
         <v>2.0</v>
       </c>
       <c r="B43" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C43" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D43" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="E43" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="F43" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G43" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H43" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I43" t="n">
-        <v>30.0</v>
+        <v>70.0</v>
       </c>
       <c r="J43" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="K43" t="n">
         <v>44375.0</v>
@@ -2764,48 +2779,48 @@
         <v>22</v>
       </c>
       <c r="M43" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="N43" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="O43" t="n">
         <v>0.0</v>
       </c>
       <c r="P43" t="n">
-        <v>46.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B44" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="F44" t="n">
         <v>2.0</v>
       </c>
       <c r="G44" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="H44" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I44" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="J44" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K44" t="n">
         <v>44375.0</v>
@@ -2814,16 +2829,16 @@
         <v>22</v>
       </c>
       <c r="M44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="N44" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="O44" t="n">
         <v>0.0</v>
       </c>
       <c r="P44" t="n">
-        <v>49.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="45">
@@ -2834,28 +2849,28 @@
         <v>2.0</v>
       </c>
       <c r="C45" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D45" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E45" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F45" t="n">
         <v>1.0</v>
       </c>
       <c r="G45" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H45" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I45" t="n">
-        <v>70.0</v>
+        <v>150.0</v>
       </c>
       <c r="J45" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="K45" t="n">
         <v>44375.0</v>
@@ -2864,16 +2879,16 @@
         <v>22</v>
       </c>
       <c r="M45" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="N45" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="O45" t="n">
         <v>0.0</v>
       </c>
       <c r="P45" t="n">
-        <v>14.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="46">
@@ -2884,46 +2899,46 @@
         <v>1.0</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>158</v>
+        <v>18</v>
       </c>
       <c r="F46" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G46" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="H46" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I46" t="n">
         <v>0.0</v>
       </c>
       <c r="J46" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="K46" t="n">
         <v>44376.0</v>
       </c>
       <c r="L46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M46" t="s">
         <v>23</v>
       </c>
       <c r="N46" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="O46" t="n">
         <v>0.0</v>
       </c>
       <c r="P46" t="n">
-        <v>54.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="47">
@@ -2934,96 +2949,96 @@
         <v>1.0</v>
       </c>
       <c r="C47" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="E47" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F47" t="n">
         <v>1.0</v>
       </c>
       <c r="G47" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H47" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I47" t="n">
-        <v>62.0</v>
+        <v>84.0</v>
       </c>
       <c r="J47" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="K47" t="n">
         <v>44376.0</v>
       </c>
       <c r="L47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M47" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="N47" t="s">
-        <v>66</v>
+        <v>166</v>
       </c>
       <c r="O47" t="n">
         <v>0.0</v>
       </c>
       <c r="P47" t="n">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B48" t="n">
         <v>1.0</v>
       </c>
       <c r="C48" t="s">
-        <v>159</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>160</v>
+        <v>47</v>
       </c>
       <c r="E48" t="s">
-        <v>161</v>
+        <v>48</v>
       </c>
       <c r="F48" t="n">
         <v>1.0</v>
       </c>
       <c r="G48" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H48" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I48" t="n">
-        <v>140.0</v>
+        <v>67.0</v>
       </c>
       <c r="J48" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="K48" t="n">
         <v>44376.0</v>
       </c>
       <c r="L48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M48" t="s">
-        <v>66</v>
+        <v>166</v>
       </c>
       <c r="N48" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="O48" t="n">
         <v>0.0</v>
       </c>
       <c r="P48" t="n">
-        <v>40.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="49">
@@ -3031,199 +3046,199 @@
         <v>2.0</v>
       </c>
       <c r="B49" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E49" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F49" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G49" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H49" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I49" t="n">
-        <v>61.0</v>
+        <v>0.0</v>
       </c>
       <c r="J49" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="K49" t="n">
         <v>44377.0</v>
       </c>
       <c r="L49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M49" t="s">
         <v>23</v>
       </c>
       <c r="N49" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="O49" t="n">
         <v>0.0</v>
       </c>
       <c r="P49" t="n">
-        <v>7.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B50" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C50" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="E50" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="F50" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G50" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H50" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I50" t="n">
-        <v>0.0</v>
+        <v>140.0</v>
       </c>
       <c r="J50" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="K50" t="n">
         <v>44377.0</v>
       </c>
       <c r="L50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M50" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="N50" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="O50" t="n">
         <v>0.0</v>
       </c>
       <c r="P50" t="n">
-        <v>22.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B51" t="n">
         <v>2.0</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="E51" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="F51" t="n">
         <v>2.0</v>
       </c>
       <c r="G51" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H51" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I51" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="J51" t="s">
-        <v>28</v>
+        <v>139</v>
       </c>
       <c r="K51" t="n">
         <v>44377.0</v>
       </c>
       <c r="L51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M51" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="N51" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="O51" t="n">
         <v>0.0</v>
       </c>
       <c r="P51" t="n">
-        <v>32.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B52" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="D52" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="E52" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F52" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G52" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H52" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I52" t="n">
-        <v>80.0</v>
+        <v>11.0</v>
       </c>
       <c r="J52" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="K52" t="n">
         <v>44378.0</v>
       </c>
       <c r="L52" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M52" t="s">
         <v>23</v>
       </c>
       <c r="N52" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="O52" t="n">
         <v>0.0</v>
       </c>
       <c r="P52" t="n">
-        <v>8.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="53">
@@ -3234,113 +3249,113 @@
         <v>1.0</v>
       </c>
       <c r="C53" t="s">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="D53" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="E53" t="s">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="F53" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G53" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H53" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I53" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="J53" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K53" t="n">
         <v>44378.0</v>
       </c>
       <c r="L53" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M53" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="N53" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="O53" t="n">
         <v>0.0</v>
       </c>
       <c r="P53" t="n">
-        <v>42.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B54" t="n">
         <v>1.0</v>
       </c>
       <c r="C54" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E54" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F54" t="n">
         <v>1.0</v>
       </c>
       <c r="G54" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H54" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I54" t="n">
-        <v>150.0</v>
+        <v>103.0</v>
       </c>
       <c r="J54" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="K54" t="n">
         <v>44378.0</v>
       </c>
       <c r="L54" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M54" t="s">
         <v>41</v>
       </c>
       <c r="N54" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="O54" t="n">
         <v>0.0</v>
       </c>
       <c r="P54" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B55" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C55" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E55" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F55" t="n">
         <v>1.0</v>
@@ -3349,31 +3364,31 @@
         <v>19</v>
       </c>
       <c r="H55" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I55" t="n">
-        <v>44.0</v>
+        <v>0.0</v>
       </c>
       <c r="J55" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="K55" t="n">
         <v>44379.0</v>
       </c>
       <c r="L55" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M55" t="s">
         <v>23</v>
       </c>
       <c r="N55" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="O55" t="n">
         <v>0.0</v>
       </c>
       <c r="P55" t="n">
-        <v>38.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="56">
@@ -3384,96 +3399,96 @@
         <v>2.0</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>180</v>
       </c>
       <c r="D56" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="E56" t="s">
-        <v>113</v>
+        <v>182</v>
       </c>
       <c r="F56" t="n">
         <v>1.0</v>
       </c>
       <c r="G56" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H56" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I56" t="n">
-        <v>60.0</v>
+        <v>61.0</v>
       </c>
       <c r="J56" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K56" t="n">
         <v>44379.0</v>
       </c>
       <c r="L56" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M56" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="N56" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="O56" t="n">
         <v>0.0</v>
       </c>
       <c r="P56" t="n">
-        <v>39.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B57" t="n">
         <v>2.0</v>
       </c>
       <c r="C57" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="D57" t="s">
-        <v>178</v>
+        <v>126</v>
       </c>
       <c r="E57" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="F57" t="n">
         <v>1.0</v>
       </c>
       <c r="G57" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H57" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="I57" t="n">
         <v>0.0</v>
       </c>
       <c r="J57" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="K57" t="n">
         <v>44379.0</v>
       </c>
       <c r="L57" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="M57" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N57" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="O57" t="n">
         <v>0.0</v>
       </c>
       <c r="P57" t="n">
-        <v>5.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="58">
@@ -3484,28 +3499,28 @@
         <v>1.0</v>
       </c>
       <c r="C58" t="s">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="D58" t="s">
-        <v>181</v>
+        <v>33</v>
       </c>
       <c r="E58" t="s">
-        <v>182</v>
+        <v>34</v>
       </c>
       <c r="F58" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G58" t="s">
         <v>19</v>
       </c>
       <c r="H58" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="I58" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J58" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="K58" t="n">
         <v>44382.0</v>
@@ -3517,13 +3532,13 @@
         <v>23</v>
       </c>
       <c r="N58" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="O58" t="n">
         <v>0.0</v>
       </c>
       <c r="P58" t="n">
-        <v>11.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="59">
@@ -3534,28 +3549,28 @@
         <v>1.0</v>
       </c>
       <c r="C59" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="D59" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="E59" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F59" t="n">
         <v>2.0</v>
       </c>
       <c r="G59" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="H59" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I59" t="n">
         <v>79.0</v>
       </c>
       <c r="J59" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K59" t="n">
         <v>44382.0</v>
@@ -3564,10 +3579,10 @@
         <v>22</v>
       </c>
       <c r="M59" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="N59" t="s">
-        <v>29</v>
+        <v>186</v>
       </c>
       <c r="O59" t="n">
         <v>0.0</v>
@@ -3578,34 +3593,34 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B60" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C60" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="D60" t="s">
-        <v>31</v>
+        <v>188</v>
       </c>
       <c r="E60" t="s">
-        <v>32</v>
+        <v>189</v>
       </c>
       <c r="F60" t="n">
         <v>1.0</v>
       </c>
       <c r="G60" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="H60" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I60" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J60" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K60" t="n">
         <v>44382.0</v>
@@ -3614,116 +3629,116 @@
         <v>22</v>
       </c>
       <c r="M60" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N60" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="O60" t="n">
         <v>0.0</v>
       </c>
       <c r="P60" t="n">
-        <v>31.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B61" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C61" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="E61" t="s">
-        <v>173</v>
+        <v>27</v>
       </c>
       <c r="F61" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G61" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H61" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I61" t="n">
-        <v>79.0</v>
+        <v>100.0</v>
       </c>
       <c r="J61" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K61" t="n">
         <v>44383.0</v>
       </c>
       <c r="L61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M61" t="s">
         <v>23</v>
       </c>
       <c r="N61" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O61" t="n">
         <v>0.0</v>
       </c>
       <c r="P61" t="n">
-        <v>37.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B62" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C62" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D62" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="E62" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="F62" t="n">
         <v>1.0</v>
       </c>
       <c r="G62" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H62" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I62" t="n">
-        <v>70.0</v>
+        <v>116.0</v>
       </c>
       <c r="J62" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="K62" t="n">
         <v>44383.0</v>
       </c>
       <c r="L62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M62" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N62" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="O62" t="n">
         <v>0.0</v>
       </c>
       <c r="P62" t="n">
-        <v>52.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="63">
@@ -3731,49 +3746,49 @@
         <v>1.0</v>
       </c>
       <c r="B63" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>183</v>
       </c>
       <c r="D63" t="s">
-        <v>126</v>
+        <v>184</v>
       </c>
       <c r="E63" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
       <c r="F63" t="n">
         <v>1.0</v>
       </c>
       <c r="G63" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H63" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I63" t="n">
-        <v>0.0</v>
+        <v>80.0</v>
       </c>
       <c r="J63" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="K63" t="n">
         <v>44383.0</v>
       </c>
       <c r="L63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M63" t="s">
         <v>41</v>
       </c>
       <c r="N63" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="O63" t="n">
         <v>0.0</v>
       </c>
       <c r="P63" t="n">
-        <v>23.0</v>
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eveything but the Parsers and DataHandler with javadoc.
</commit_message>
<xml_diff>
--- a/files/output/prueba.xlsx
+++ b/files/output/prueba.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="192">
   <si>
     <t>Curso</t>
   </si>
@@ -62,6 +62,324 @@
     <t>ID</t>
   </si>
   <si>
+    <t>GIISOF01-1-005</t>
+  </si>
+  <si>
+    <t>OyE</t>
+  </si>
+  <si>
+    <t>Ondas y Electromagnetismo</t>
+  </si>
+  <si>
+    <t>Teórico</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>3:00:00</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>9:00:00</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-005</t>
+  </si>
+  <si>
+    <t>ASLEPI</t>
+  </si>
+  <si>
+    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
+  </si>
+  <si>
+    <t>No presencial</t>
+  </si>
+  <si>
+    <t>1:00:00</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-011</t>
+  </si>
+  <si>
+    <t>IFA</t>
+  </si>
+  <si>
+    <t>Informática Forense y Auditoría</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-006</t>
+  </si>
+  <si>
+    <t>SSOO</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos</t>
+  </si>
+  <si>
+    <t>Práctico</t>
+  </si>
+  <si>
+    <t>19:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-002</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Ingeniería de Requisitos</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-008</t>
+  </si>
+  <si>
+    <t>FCR</t>
+  </si>
+  <si>
+    <t>Fundamentos de Computadores y Redes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-005 </t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>Sistemas Distribuidos e Internet</t>
+  </si>
+  <si>
+    <t>1:30:00</t>
+  </si>
+  <si>
+    <t>16:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-005</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>Computabilidad</t>
+  </si>
+  <si>
+    <t>19:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-0-015 </t>
+  </si>
+  <si>
+    <t>SIW</t>
+  </si>
+  <si>
+    <t>Sistemas de Información para la Web</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>0:30:00</t>
+  </si>
+  <si>
+    <t>miércoles</t>
+  </si>
+  <si>
+    <t>9:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-007</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Introducción a la Programación</t>
+  </si>
+  <si>
+    <t>2:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-002</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Arquitectura de Computadores</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-010 </t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Seguridad de Sistemas Informáticos</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-016</t>
+  </si>
+  <si>
+    <t>SEV</t>
+  </si>
+  <si>
+    <t>Software de entretenimiento y videojuegos</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-008</t>
+  </si>
+  <si>
+    <t>BBDD</t>
+  </si>
+  <si>
+    <t>Bases de Datos</t>
+  </si>
+  <si>
+    <t>12:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-009 </t>
+  </si>
+  <si>
+    <t>Computación Numérica</t>
+  </si>
+  <si>
+    <t>15:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-010</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-001</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática</t>
+  </si>
+  <si>
+    <t>2:00:00</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-007 </t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>Comunicación Persona-Máquina</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-004</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Diseño del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-017</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Software para Robots</t>
+  </si>
+  <si>
+    <t>18:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-009</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-009</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>Autómatas y Matemáticas Discretas</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-001</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Repositorios de Información</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-018</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Informática Audiovisual</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-003</t>
+  </si>
+  <si>
+    <t>CVVS</t>
+  </si>
+  <si>
+    <t>Calidad, Validación y Verificación del Software</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-005</t>
+  </si>
+  <si>
     <t>GIISOF01-0-013</t>
   </si>
   <si>
@@ -71,57 +389,132 @@
     <t>Software para Dispositivos Móviles</t>
   </si>
   <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
-    <t>Entrega</t>
-  </si>
-  <si>
-    <t>0:30:00</t>
-  </si>
-  <si>
-    <t>lunes</t>
-  </si>
-  <si>
-    <t>9:00:00</t>
-  </si>
-  <si>
-    <t>9:30:00</t>
+    <t>GIISOF01-2-007</t>
+  </si>
+  <si>
+    <t>13:30:00</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-008 </t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Arquitectura del Software</t>
+  </si>
+  <si>
+    <t>Presentación</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-008</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Sistemas Inteligentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-009 </t>
+  </si>
+  <si>
+    <t>DLP</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
+  </si>
+  <si>
+    <t>3:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-010</t>
+  </si>
+  <si>
+    <t>Alg</t>
+  </si>
+  <si>
+    <t>Algoritmia</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-002</t>
+  </si>
+  <si>
+    <t>SEW</t>
+  </si>
+  <si>
+    <t>Software y Estándares para la Web</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-002</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Álgebra Lineal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-002 </t>
+  </si>
+  <si>
+    <t>GIISOF01-1-003</t>
+  </si>
+  <si>
+    <t>Emp</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-004</t>
+  </si>
+  <si>
+    <t>DPPI</t>
+  </si>
+  <si>
+    <t>Dirección y Planificación de Proyectos Informáticos</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-001</t>
+  </si>
+  <si>
+    <t>TEC</t>
+  </si>
+  <si>
+    <t>Tecnología Electrónica de Computadores</t>
+  </si>
+  <si>
+    <t>18:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-004</t>
+  </si>
+  <si>
+    <t>TPP</t>
+  </si>
+  <si>
+    <t>Tecnología y Paradigmas de Programación</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-004 </t>
+  </si>
+  <si>
+    <t>GIISOF01-3-008</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática (80)</t>
   </si>
   <si>
     <t xml:space="preserve">GIISOF01-2-010 </t>
   </si>
   <si>
-    <t>Alg</t>
-  </si>
-  <si>
-    <t>Algoritmia</t>
-  </si>
-  <si>
-    <t>Práctico</t>
-  </si>
-  <si>
-    <t>Presencial</t>
-  </si>
-  <si>
-    <t>2:00:00</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-002 </t>
-  </si>
-  <si>
-    <t>SEW</t>
-  </si>
-  <si>
-    <t>Software y Estándares para la Web</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
     <t>GIISOF01-1-006</t>
   </si>
   <si>
@@ -131,100 +524,40 @@
     <t>Estadística</t>
   </si>
   <si>
-    <t>Teórico</t>
-  </si>
-  <si>
-    <t>3:00:00</t>
-  </si>
-  <si>
-    <t>15:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-002</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>Álgebra Lineal</t>
-  </si>
-  <si>
-    <t>martes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-001</t>
-  </si>
-  <si>
-    <t>RI</t>
-  </si>
-  <si>
-    <t>Repositorios de Información</t>
-  </si>
-  <si>
-    <t>12:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-006</t>
-  </si>
-  <si>
-    <t>SSOO</t>
-  </si>
-  <si>
-    <t>Sistemas Operativos</t>
-  </si>
-  <si>
-    <t>1:00:00</t>
-  </si>
-  <si>
-    <t>13:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-008</t>
-  </si>
-  <si>
-    <t>BBDD</t>
-  </si>
-  <si>
-    <t>Bases de Datos</t>
-  </si>
-  <si>
-    <t>2:30:00</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t>miércoles</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-009</t>
-  </si>
-  <si>
-    <t>Computación Numérica</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-004</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>Diseño del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-004</t>
-  </si>
-  <si>
-    <t>DPPI</t>
-  </si>
-  <si>
-    <t>Dirección y Planificación de Proyectos Informáticos</t>
-  </si>
-  <si>
-    <t>No presencial</t>
-  </si>
-  <si>
-    <t>20:00:00</t>
+    <t>GIISOF01-2-003</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Estructura de Datos</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-004</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Cálculo</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-003</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>Ingeniería del Proceso Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-006</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Administración de Sistemas y Redes</t>
   </si>
   <si>
     <t>GIISOF01-0-010</t>
@@ -236,361 +569,25 @@
     <t>Integración de aplicaciones empresariales</t>
   </si>
   <si>
-    <t>jueves</t>
-  </si>
-  <si>
-    <t>10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-015 </t>
-  </si>
-  <si>
-    <t>SIW</t>
-  </si>
-  <si>
-    <t>Sistemas de Información para la Web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-004 </t>
-  </si>
-  <si>
-    <t>GIISOF01-2-002</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Arquitectura de Computadores</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-003</t>
-  </si>
-  <si>
-    <t>CVVS</t>
-  </si>
-  <si>
-    <t>Calidad, Validación y Verificación del Software</t>
-  </si>
-  <si>
-    <t>viernes</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-009</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>GIISOF01-2-001</t>
-  </si>
-  <si>
-    <t>TEC</t>
-  </si>
-  <si>
-    <t>Tecnología Electrónica de Computadores</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-003</t>
-  </si>
-  <si>
-    <t>IPS</t>
-  </si>
-  <si>
-    <t>Ingeniería del Proceso Software</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-005</t>
-  </si>
-  <si>
-    <t>ASLEPI</t>
-  </si>
-  <si>
-    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-003</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>Estructura de Datos</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-007</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Introducción a la Programación</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-008 </t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>Presentación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-009 </t>
-  </si>
-  <si>
-    <t>DLP</t>
+    <t xml:space="preserve">GIISOF01-0-013 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-001 </t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-010</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Metodología de la Programación</t>
   </si>
   <si>
     <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
-  </si>
-  <si>
-    <t>3:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-009 </t>
-  </si>
-  <si>
-    <t>15:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-016</t>
-  </si>
-  <si>
-    <t>SEV</t>
-  </si>
-  <si>
-    <t>Software de entretenimiento y videojuegos</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-010</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>Metodología de la Programación</t>
-  </si>
-  <si>
-    <t>19:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-008</t>
-  </si>
-  <si>
-    <t>FCR</t>
-  </si>
-  <si>
-    <t>Fundamentos de Computadores y Redes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-005</t>
-  </si>
-  <si>
-    <t>SDI</t>
-  </si>
-  <si>
-    <t>Sistemas Distribuidos e Internet</t>
-  </si>
-  <si>
-    <t>17:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-017</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>Software para Robots</t>
-  </si>
-  <si>
-    <t>Autómatas y Matemáticas Discretas</t>
-  </si>
-  <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-001 </t>
-  </si>
-  <si>
-    <t>GIISOF01-3-002</t>
-  </si>
-  <si>
-    <t>1:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-011</t>
-  </si>
-  <si>
-    <t>IFA</t>
-  </si>
-  <si>
-    <t>Informática Forense y Auditoría</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-010 </t>
-  </si>
-  <si>
-    <t>SSI</t>
-  </si>
-  <si>
-    <t>Seguridad de Sistemas Informáticos</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-002</t>
-  </si>
-  <si>
-    <t>IR</t>
-  </si>
-  <si>
-    <t>Ingeniería de Requisitos</t>
-  </si>
-  <si>
-    <t>18:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-003</t>
-  </si>
-  <si>
-    <t>Emp</t>
-  </si>
-  <si>
-    <t>Empresa</t>
-  </si>
-  <si>
-    <t>20:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-008</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-005</t>
-  </si>
-  <si>
-    <t>Comp</t>
-  </si>
-  <si>
-    <t>Computabilidad</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-005</t>
-  </si>
-  <si>
-    <t>OyE</t>
-  </si>
-  <si>
-    <t>Ondas y Electromagnetismo</t>
-  </si>
-  <si>
-    <t>18:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-013 </t>
-  </si>
-  <si>
-    <t>GIISOF01-2-007</t>
-  </si>
-  <si>
-    <t>CPM</t>
-  </si>
-  <si>
-    <t>Comunicación Persona-Máquina</t>
-  </si>
-  <si>
-    <t>10:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-007 </t>
-  </si>
-  <si>
-    <t>GIISOF01-1-004</t>
-  </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Cálculo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-005 </t>
-  </si>
-  <si>
-    <t>16:30:00</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-008</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Sistemas Inteligentes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-006</t>
-  </si>
-  <si>
-    <t>ASR</t>
-  </si>
-  <si>
-    <t>Administración de Sistemas y Redes</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-004</t>
-  </si>
-  <si>
-    <t>TPP</t>
-  </si>
-  <si>
-    <t>Tecnología y Paradigmas de Programación</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-001</t>
-  </si>
-  <si>
-    <t>FI</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática (80)</t>
-  </si>
-  <si>
-    <t>14:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-018</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>Informática Audiovisual</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-010</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-010</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática</t>
   </si>
 </sst>
 </file>
@@ -693,10 +690,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -717,7 +714,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0</v>
+        <v>150.0</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -735,15 +732,15 @@
         <v>24</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P2" t="n">
-        <v>3.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B3" t="n">
         <v>2.0</v>
@@ -758,19 +755,19 @@
         <v>27</v>
       </c>
       <c r="F3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="J3" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
       </c>
       <c r="K3" t="n">
         <v>44361.0</v>
@@ -782,45 +779,45 @@
         <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P3" t="n">
-        <v>46.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B4" t="n">
         <v>1.0</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K4" t="n">
         <v>44361.0</v>
@@ -829,21 +826,21 @@
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
         <v>35</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P4" t="n">
-        <v>34.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B5" t="n">
         <v>2.0</v>
@@ -864,13 +861,13 @@
         <v>39</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I5" t="n">
-        <v>183.0</v>
+        <v>40.0</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K5" t="n">
         <v>44361.0</v>
@@ -882,92 +879,92 @@
         <v>35</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P5" t="n">
-        <v>47.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
       </c>
       <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
       <c r="F6" t="n">
         <v>1.0</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I6" t="n">
-        <v>120.0</v>
+        <v>90.0</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K6" t="n">
         <v>44362.0</v>
       </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M6" t="s">
         <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P6" t="n">
-        <v>56.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
       <c r="F7" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="J7" t="s">
         <v>21</v>
@@ -976,69 +973,69 @@
         <v>44362.0</v>
       </c>
       <c r="L7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="N7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B8" t="n">
         <v>2.0</v>
       </c>
       <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
-      </c>
       <c r="F8" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G8" t="s">
         <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K8" t="n">
         <v>44362.0</v>
       </c>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="N8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P8" t="n">
-        <v>1.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="9">
@@ -1046,116 +1043,116 @@
         <v>2.0</v>
       </c>
       <c r="B9" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
         <v>55</v>
       </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" t="s">
-        <v>57</v>
-      </c>
       <c r="F9" t="n">
         <v>1.0</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I9" t="n">
-        <v>71.0</v>
+        <v>70.0</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="K9" t="n">
         <v>44362.0</v>
       </c>
       <c r="L9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M9" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="N9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P9" t="n">
-        <v>55.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B10" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F10" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="I10" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J10" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="K10" t="n">
         <v>44363.0</v>
       </c>
       <c r="L10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M10" t="s">
         <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="O10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P10" t="n">
-        <v>31.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F11" t="n">
         <v>1.0</v>
@@ -1164,131 +1161,131 @@
         <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I11" t="n">
         <v>50.0</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="K11" t="n">
         <v>44363.0</v>
       </c>
       <c r="L11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M11" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P11" t="n">
-        <v>18.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B12" t="n">
         <v>1.0</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F12" t="n">
         <v>1.0</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I12" t="n">
-        <v>150.0</v>
+        <v>60.0</v>
       </c>
       <c r="J12" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="K12" t="n">
         <v>44363.0</v>
       </c>
       <c r="L12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M12" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="N12" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P12" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B13" t="n">
         <v>2.0</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F13" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G13" t="s">
         <v>39</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I13" t="n">
-        <v>120.0</v>
+        <v>71.0</v>
       </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="K13" t="n">
         <v>44363.0</v>
       </c>
       <c r="L13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M13" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P13" t="n">
-        <v>45.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="14">
@@ -1299,428 +1296,428 @@
         <v>1.0</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F14" t="n">
         <v>1.0</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="I14" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="K14" t="n">
         <v>44364.0</v>
       </c>
       <c r="L14" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M14" t="s">
         <v>23</v>
       </c>
       <c r="N14" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P14" t="n">
-        <v>25.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F15" t="n">
         <v>1.0</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="J15" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K15" t="n">
         <v>44364.0</v>
       </c>
       <c r="L15" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P15" t="n">
-        <v>19.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="F16" t="n">
         <v>2.0</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I16" t="n">
-        <v>79.0</v>
+        <v>50.0</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K16" t="n">
         <v>44364.0</v>
       </c>
       <c r="L16" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M16" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P16" t="n">
-        <v>37.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B17" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F17" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G17" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I17" t="n">
-        <v>60.0</v>
+        <v>116.0</v>
       </c>
       <c r="J17" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K17" t="n">
         <v>44364.0</v>
       </c>
       <c r="L17" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M17" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="N17" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="O17" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P17" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="B18" t="n">
         <v>1.0</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F18" t="n">
         <v>1.0</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I18" t="n">
-        <v>45.0</v>
+        <v>80.0</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="K18" t="n">
         <v>44365.0</v>
       </c>
       <c r="L18" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M18" t="s">
         <v>23</v>
       </c>
       <c r="N18" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P18" t="n">
-        <v>30.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="F19" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G19" t="s">
         <v>39</v>
       </c>
       <c r="H19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I19" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="J19" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K19" t="n">
         <v>44365.0</v>
       </c>
       <c r="L19" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M19" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="N19" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P19" t="n">
-        <v>14.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B20" t="n">
         <v>1.0</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F20" t="n">
         <v>1.0</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I20" t="n">
-        <v>8.0</v>
+        <v>150.0</v>
       </c>
       <c r="J20" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="K20" t="n">
         <v>44365.0</v>
       </c>
       <c r="L20" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N20" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="O20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P20" t="n">
-        <v>57.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B21" t="n">
         <v>1.0</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="F21" t="n">
         <v>1.0</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="I21" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J21" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="K21" t="n">
         <v>44365.0</v>
       </c>
       <c r="L21" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M21" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="N21" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P21" t="n">
-        <v>11.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B22" t="n">
         <v>2.0</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F22" t="n">
         <v>1.0</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I22" t="n">
-        <v>177.0</v>
+        <v>50.0</v>
       </c>
       <c r="J22" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="K22" t="n">
         <v>44368.0</v>
@@ -1732,45 +1729,45 @@
         <v>23</v>
       </c>
       <c r="N22" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P22" t="n">
-        <v>53.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B23" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E23" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F23" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G23" t="s">
         <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I23" t="n">
-        <v>62.0</v>
+        <v>70.0</v>
       </c>
       <c r="J23" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="K23" t="n">
         <v>44368.0</v>
@@ -1779,48 +1776,48 @@
         <v>22</v>
       </c>
       <c r="M23" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="N23" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P23" t="n">
-        <v>12.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B24" t="n">
         <v>1.0</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
       </c>
       <c r="G24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" t="s">
         <v>28</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="J24" t="s">
         <v>29</v>
-      </c>
-      <c r="I24" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>58</v>
       </c>
       <c r="K24" t="n">
         <v>44368.0</v>
@@ -1829,48 +1826,48 @@
         <v>22</v>
       </c>
       <c r="M24" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" t="s">
         <v>35</v>
       </c>
-      <c r="N24" t="s">
-        <v>107</v>
-      </c>
       <c r="O24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P24" t="n">
-        <v>44.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E25" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="H25" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="I25" t="n">
         <v>0.0</v>
       </c>
       <c r="J25" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="K25" t="n">
         <v>44368.0</v>
@@ -1879,116 +1876,116 @@
         <v>22</v>
       </c>
       <c r="M25" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N25" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="O25" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P25" t="n">
-        <v>22.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B26" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E26" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F26" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="J26" t="s">
         <v>29</v>
-      </c>
-      <c r="I26" t="n">
-        <v>89.0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>115</v>
       </c>
       <c r="K26" t="n">
         <v>44369.0</v>
       </c>
       <c r="L26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M26" t="s">
         <v>23</v>
       </c>
       <c r="N26" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P26" t="n">
-        <v>58.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B27" t="n">
         <v>2.0</v>
       </c>
       <c r="C27" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F27" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G27" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I27" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="J27" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="K27" t="n">
         <v>44369.0</v>
       </c>
       <c r="L27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M27" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="N27" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="O27" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P27" t="n">
-        <v>49.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="28">
@@ -1999,96 +1996,96 @@
         <v>1.0</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E28" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F28" t="n">
         <v>1.0</v>
       </c>
       <c r="G28" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="H28" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="I28" t="n">
         <v>0.0</v>
       </c>
       <c r="J28" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="K28" t="n">
         <v>44369.0</v>
       </c>
       <c r="L28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M28" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="N28" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="O28" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P28" t="n">
-        <v>54.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B29" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F29" t="n">
         <v>1.0</v>
       </c>
       <c r="G29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" t="s">
         <v>28</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="J29" t="s">
         <v>29</v>
-      </c>
-      <c r="I29" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>40</v>
       </c>
       <c r="K29" t="n">
         <v>44369.0</v>
       </c>
       <c r="L29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M29" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="N29" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P29" t="n">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="30">
@@ -2099,151 +2096,151 @@
         <v>2.0</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E30" t="s">
         <v>127</v>
       </c>
       <c r="F30" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G30" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H30" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I30" t="n">
-        <v>20.0</v>
+        <v>70.0</v>
       </c>
       <c r="J30" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="K30" t="n">
         <v>44370.0</v>
       </c>
       <c r="L30" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M30" t="s">
         <v>23</v>
       </c>
       <c r="N30" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="O30" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P30" t="n">
-        <v>61.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B31" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="F31" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="H31" t="s">
+        <v>131</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J31" t="s">
         <v>29</v>
-      </c>
-      <c r="I31" t="n">
-        <v>62.0</v>
-      </c>
-      <c r="J31" t="s">
-        <v>40</v>
       </c>
       <c r="K31" t="n">
         <v>44370.0</v>
       </c>
       <c r="L31" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M31" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="N31" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="O31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P31" t="n">
-        <v>35.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B32" t="n">
         <v>2.0</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="F32" t="n">
         <v>1.0</v>
       </c>
       <c r="G32" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H32" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I32" t="n">
         <v>40.0</v>
       </c>
       <c r="J32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K32" t="n">
         <v>44370.0</v>
       </c>
       <c r="L32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M32" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="N32" t="s">
-        <v>131</v>
+        <v>30</v>
       </c>
       <c r="O32" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P32" t="n">
-        <v>15.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="B33" t="n">
         <v>1.0</v>
@@ -2267,78 +2264,78 @@
         <v>20</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0</v>
+        <v>103.0</v>
       </c>
       <c r="J33" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="K33" t="n">
         <v>44370.0</v>
       </c>
       <c r="L33" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M33" t="s">
-        <v>131</v>
+        <v>34</v>
       </c>
       <c r="N33" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P33" t="n">
-        <v>50.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B34" t="n">
         <v>2.0</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F34" t="n">
         <v>2.0</v>
       </c>
       <c r="G34" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H34" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I34" t="n">
-        <v>70.0</v>
+        <v>11.0</v>
       </c>
       <c r="J34" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="K34" t="n">
         <v>44371.0</v>
       </c>
       <c r="L34" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M34" t="s">
         <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P34" t="n">
-        <v>32.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="35">
@@ -2346,49 +2343,49 @@
         <v>2.0</v>
       </c>
       <c r="B35" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>141</v>
       </c>
       <c r="F35" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G35" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H35" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I35" t="n">
-        <v>8.0</v>
+        <v>100.0</v>
       </c>
       <c r="J35" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="K35" t="n">
         <v>44371.0</v>
       </c>
       <c r="L35" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M35" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="N35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P35" t="n">
-        <v>59.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="36">
@@ -2399,43 +2396,43 @@
         <v>1.0</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="F36" t="n">
         <v>1.0</v>
       </c>
       <c r="G36" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H36" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="I36" t="n">
         <v>0.0</v>
       </c>
       <c r="J36" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="K36" t="n">
         <v>44371.0</v>
       </c>
       <c r="L36" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P36" t="n">
         <v>33.0</v>
@@ -2443,152 +2440,152 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B37" t="n">
         <v>1.0</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="E37" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F37" t="n">
         <v>1.0</v>
       </c>
       <c r="G37" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H37" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I37" t="n">
-        <v>3.0</v>
+        <v>120.0</v>
       </c>
       <c r="J37" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="K37" t="n">
         <v>44371.0</v>
       </c>
       <c r="L37" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M37" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="N37" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="O37" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P37" t="n">
-        <v>41.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B38" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>143</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="F38" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G38" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="H38" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="I38" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="J38" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K38" t="n">
         <v>44372.0</v>
       </c>
       <c r="L38" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M38" t="s">
         <v>23</v>
       </c>
       <c r="N38" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="O38" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P38" t="n">
-        <v>39.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B39" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C39" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E39" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F39" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I39" t="n">
-        <v>71.0</v>
+        <v>44.0</v>
       </c>
       <c r="J39" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="K39" t="n">
         <v>44372.0</v>
       </c>
       <c r="L39" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M39" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="N39" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="O39" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P39" t="n">
-        <v>51.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="40">
@@ -2596,116 +2593,116 @@
         <v>4.0</v>
       </c>
       <c r="B40" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C40" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D40" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="F40" t="n">
         <v>1.0</v>
       </c>
       <c r="G40" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I40" t="n">
-        <v>90.0</v>
+        <v>120.0</v>
       </c>
       <c r="J40" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="K40" t="n">
         <v>44372.0</v>
       </c>
       <c r="L40" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M40" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N40" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P40" t="n">
-        <v>10.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B41" t="n">
         <v>1.0</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D41" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E41" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="F41" t="n">
         <v>1.0</v>
       </c>
       <c r="G41" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H41" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J41" t="s">
         <v>29</v>
-      </c>
-      <c r="I41" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>58</v>
       </c>
       <c r="K41" t="n">
         <v>44372.0</v>
       </c>
       <c r="L41" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M41" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="N41" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P41" t="n">
-        <v>38.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B42" t="n">
         <v>2.0</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>160</v>
       </c>
       <c r="E42" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
@@ -2714,13 +2711,13 @@
         <v>39</v>
       </c>
       <c r="H42" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0</v>
+        <v>61.0</v>
       </c>
       <c r="J42" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="K42" t="n">
         <v>44375.0</v>
@@ -2732,45 +2729,45 @@
         <v>23</v>
       </c>
       <c r="N42" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
       <c r="O42" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P42" t="n">
-        <v>21.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B43" t="n">
         <v>1.0</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D43" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="E43" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
       <c r="F43" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G43" t="s">
         <v>39</v>
       </c>
       <c r="H43" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I43" t="n">
-        <v>70.0</v>
+        <v>79.0</v>
       </c>
       <c r="J43" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K43" t="n">
         <v>44375.0</v>
@@ -2779,48 +2776,48 @@
         <v>22</v>
       </c>
       <c r="M43" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
       <c r="N43" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="O43" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P43" t="n">
-        <v>52.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B44" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="F44" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G44" t="s">
         <v>19</v>
       </c>
       <c r="H44" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I44" t="n">
         <v>0.0</v>
       </c>
       <c r="J44" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K44" t="n">
         <v>44375.0</v>
@@ -2829,16 +2826,16 @@
         <v>22</v>
       </c>
       <c r="M44" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N44" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P44" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="45">
@@ -2846,31 +2843,31 @@
         <v>1.0</v>
       </c>
       <c r="B45" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="E45" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F45" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G45" t="s">
         <v>39</v>
       </c>
       <c r="H45" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I45" t="n">
-        <v>150.0</v>
+        <v>79.0</v>
       </c>
       <c r="J45" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="K45" t="n">
         <v>44375.0</v>
@@ -2879,116 +2876,116 @@
         <v>22</v>
       </c>
       <c r="M45" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="N45" t="s">
-        <v>161</v>
+        <v>106</v>
       </c>
       <c r="O45" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P45" t="n">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B46" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C46" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>141</v>
       </c>
       <c r="F46" t="n">
         <v>2.0</v>
       </c>
       <c r="G46" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H46" t="s">
         <v>20</v>
       </c>
       <c r="I46" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="J46" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="K46" t="n">
         <v>44376.0</v>
       </c>
       <c r="L46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M46" t="s">
         <v>23</v>
       </c>
       <c r="N46" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P46" t="n">
-        <v>13.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B47" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E47" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F47" t="n">
         <v>1.0</v>
       </c>
       <c r="G47" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H47" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I47" t="n">
-        <v>84.0</v>
+        <v>183.0</v>
       </c>
       <c r="J47" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="K47" t="n">
         <v>44376.0</v>
       </c>
       <c r="L47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M47" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="N47" t="s">
-        <v>166</v>
+        <v>99</v>
       </c>
       <c r="O47" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P47" t="n">
-        <v>16.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="48">
@@ -2999,46 +2996,46 @@
         <v>1.0</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>47</v>
+        <v>143</v>
       </c>
       <c r="E48" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="F48" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G48" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="H48" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="I48" t="n">
-        <v>67.0</v>
+        <v>0.0</v>
       </c>
       <c r="J48" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="K48" t="n">
         <v>44376.0</v>
       </c>
       <c r="L48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M48" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
       <c r="N48" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="O48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P48" t="n">
-        <v>9.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="49">
@@ -3049,46 +3046,46 @@
         <v>1.0</v>
       </c>
       <c r="C49" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F49" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G49" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H49" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I49" t="n">
-        <v>0.0</v>
+        <v>62.0</v>
       </c>
       <c r="J49" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K49" t="n">
         <v>44377.0</v>
       </c>
       <c r="L49" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M49" t="s">
         <v>23</v>
       </c>
       <c r="N49" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="O49" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P49" t="n">
-        <v>42.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="50">
@@ -3099,43 +3096,43 @@
         <v>1.0</v>
       </c>
       <c r="C50" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D50" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E50" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F50" t="n">
         <v>1.0</v>
       </c>
       <c r="G50" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H50" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I50" t="n">
         <v>140.0</v>
       </c>
       <c r="J50" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="K50" t="n">
         <v>44377.0</v>
       </c>
       <c r="L50" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M50" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="N50" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="O50" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P50" t="n">
         <v>40.0</v>
@@ -3146,249 +3143,249 @@
         <v>3.0</v>
       </c>
       <c r="B51" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D51" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="E51" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="F51" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G51" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H51" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I51" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="J51" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
       <c r="K51" t="n">
         <v>44377.0</v>
       </c>
       <c r="L51" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M51" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N51" t="s">
-        <v>172</v>
+        <v>35</v>
       </c>
       <c r="O51" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P51" t="n">
-        <v>48.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B52" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="D52" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="E52" t="s">
-        <v>173</v>
+        <v>71</v>
       </c>
       <c r="F52" t="n">
         <v>2.0</v>
       </c>
       <c r="G52" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H52" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I52" t="n">
-        <v>11.0</v>
+        <v>60.0</v>
       </c>
       <c r="J52" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="K52" t="n">
         <v>44378.0</v>
       </c>
       <c r="L52" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M52" t="s">
         <v>23</v>
       </c>
       <c r="N52" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
       <c r="O52" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P52" t="n">
-        <v>60.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B53" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>179</v>
       </c>
       <c r="D53" t="s">
-        <v>81</v>
+        <v>180</v>
       </c>
       <c r="E53" t="s">
-        <v>82</v>
+        <v>181</v>
       </c>
       <c r="F53" t="n">
         <v>1.0</v>
       </c>
       <c r="G53" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="H53" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="I53" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="J53" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="K53" t="n">
         <v>44378.0</v>
       </c>
       <c r="L53" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M53" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
       <c r="N53" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="O53" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P53" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="B54" t="n">
         <v>1.0</v>
       </c>
       <c r="C54" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D54" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="E54" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="F54" t="n">
         <v>1.0</v>
       </c>
       <c r="G54" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J54" t="s">
         <v>29</v>
-      </c>
-      <c r="I54" t="n">
-        <v>103.0</v>
-      </c>
-      <c r="J54" t="s">
-        <v>58</v>
       </c>
       <c r="K54" t="n">
         <v>44378.0</v>
       </c>
       <c r="L54" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M54" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="N54" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="O54" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P54" t="n">
-        <v>6.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C55" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D55" t="s">
-        <v>178</v>
+        <v>123</v>
       </c>
       <c r="E55" t="s">
-        <v>179</v>
+        <v>124</v>
       </c>
       <c r="F55" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G55" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="H55" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="I55" t="n">
         <v>0.0</v>
       </c>
       <c r="J55" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="K55" t="n">
         <v>44379.0</v>
       </c>
       <c r="L55" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M55" t="s">
         <v>23</v>
       </c>
       <c r="N55" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="O55" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P55" t="n">
-        <v>5.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="56">
@@ -3396,49 +3393,49 @@
         <v>2.0</v>
       </c>
       <c r="B56" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C56" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D56" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="E56" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="F56" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G56" t="s">
+        <v>39</v>
+      </c>
+      <c r="H56" t="s">
         <v>28</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J56" t="s">
         <v>29</v>
-      </c>
-      <c r="I56" t="n">
-        <v>61.0</v>
-      </c>
-      <c r="J56" t="s">
-        <v>58</v>
       </c>
       <c r="K56" t="n">
         <v>44379.0</v>
       </c>
       <c r="L56" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M56" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>35</v>
+        <v>187</v>
       </c>
       <c r="O56" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P56" t="n">
-        <v>7.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="57">
@@ -3449,43 +3446,43 @@
         <v>2.0</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="E57" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="F57" t="n">
         <v>1.0</v>
       </c>
       <c r="G57" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H57" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I57" t="n">
         <v>0.0</v>
       </c>
       <c r="J57" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="K57" t="n">
         <v>44379.0</v>
       </c>
       <c r="L57" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M57" t="s">
-        <v>35</v>
+        <v>187</v>
       </c>
       <c r="N57" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="O57" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P57" t="n">
         <v>23.0</v>
@@ -3493,34 +3490,34 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B58" t="n">
         <v>1.0</v>
       </c>
       <c r="C58" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="E58" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="F58" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G58" t="s">
         <v>19</v>
       </c>
       <c r="H58" t="s">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="I58" t="n">
         <v>0.0</v>
       </c>
       <c r="J58" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="K58" t="n">
         <v>44382.0</v>
@@ -3532,45 +3529,45 @@
         <v>23</v>
       </c>
       <c r="N58" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="O58" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P58" t="n">
-        <v>43.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B59" t="n">
         <v>1.0</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D59" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="F59" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G59" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H59" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I59" t="n">
-        <v>79.0</v>
+        <v>62.0</v>
       </c>
       <c r="J59" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="K59" t="n">
         <v>44382.0</v>
@@ -3579,48 +3576,48 @@
         <v>22</v>
       </c>
       <c r="M59" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="N59" t="s">
-        <v>186</v>
+        <v>30</v>
       </c>
       <c r="O59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P59" t="n">
-        <v>29.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B60" t="n">
         <v>0.0</v>
       </c>
-      <c r="B60" t="n">
-        <v>1.0</v>
-      </c>
       <c r="C60" t="s">
-        <v>187</v>
+        <v>111</v>
       </c>
       <c r="D60" t="s">
-        <v>188</v>
+        <v>112</v>
       </c>
       <c r="E60" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="F60" t="n">
         <v>1.0</v>
       </c>
       <c r="G60" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="I60" t="n">
         <v>0.0</v>
       </c>
       <c r="J60" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="K60" t="n">
         <v>44382.0</v>
@@ -3629,33 +3626,33 @@
         <v>22</v>
       </c>
       <c r="M60" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N60" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="O60" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P60" t="n">
         <v>0.0</v>
-      </c>
-      <c r="P60" t="n">
-        <v>36.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B61" t="n">
         <v>2.0</v>
       </c>
       <c r="C61" t="s">
+        <v>188</v>
+      </c>
+      <c r="D61" t="s">
+        <v>189</v>
+      </c>
+      <c r="E61" t="s">
         <v>190</v>
-      </c>
-      <c r="D61" t="s">
-        <v>26</v>
-      </c>
-      <c r="E61" t="s">
-        <v>27</v>
       </c>
       <c r="F61" t="n">
         <v>1.0</v>
@@ -3664,48 +3661,48 @@
         <v>39</v>
       </c>
       <c r="H61" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I61" t="n">
-        <v>100.0</v>
+        <v>50.0</v>
       </c>
       <c r="J61" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="K61" t="n">
         <v>44383.0</v>
       </c>
       <c r="L61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M61" t="s">
         <v>23</v>
       </c>
       <c r="N61" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O61" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P61" t="n">
-        <v>24.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B62" t="n">
         <v>2.0</v>
       </c>
       <c r="C62" t="s">
-        <v>191</v>
+        <v>81</v>
       </c>
       <c r="D62" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="E62" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="F62" t="n">
         <v>1.0</v>
@@ -3714,81 +3711,81 @@
         <v>39</v>
       </c>
       <c r="H62" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I62" t="n">
-        <v>116.0</v>
+        <v>71.0</v>
       </c>
       <c r="J62" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="K62" t="n">
         <v>44383.0</v>
       </c>
       <c r="L62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M62" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N62" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="O62" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P62" t="n">
-        <v>27.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B63" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="D63" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="E63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F63" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G63" t="s">
         <v>39</v>
       </c>
       <c r="H63" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I63" t="n">
-        <v>80.0</v>
+        <v>89.0</v>
       </c>
       <c r="J63" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="K63" t="n">
         <v>44383.0</v>
       </c>
       <c r="L63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M63" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="N63" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="O63" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P63" t="n">
-        <v>8.0</v>
+        <v>58.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now the algorithm can provide more than one final planification.
</commit_message>
<xml_diff>
--- a/files/output/prueba.xlsx
+++ b/files/output/prueba.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="208">
   <si>
     <t>Curso</t>
   </si>
@@ -62,6 +62,138 @@
     <t>ID</t>
   </si>
   <si>
+    <t>GIISOF01-1-008</t>
+  </si>
+  <si>
+    <t>FCR</t>
+  </si>
+  <si>
+    <t>Fundamentos de Computadores y Redes</t>
+  </si>
+  <si>
+    <t>Práctico</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
+    <t>3:00:00</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>9:00:00</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-0-015 </t>
+  </si>
+  <si>
+    <t>SIW</t>
+  </si>
+  <si>
+    <t>Sistemas de Información para la Web</t>
+  </si>
+  <si>
+    <t>Trabajo</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>0:30:00</t>
+  </si>
+  <si>
+    <t>12:15:00</t>
+  </si>
+  <si>
+    <t>12:45:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-001</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>Repositorios de Información</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>15:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-006</t>
+  </si>
+  <si>
+    <t>SSOO</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos</t>
+  </si>
+  <si>
+    <t>Teórico</t>
+  </si>
+  <si>
+    <t>1:00:00</t>
+  </si>
+  <si>
+    <t>15:45:00</t>
+  </si>
+  <si>
+    <t>16:45:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-005</t>
+  </si>
+  <si>
+    <t>OyE</t>
+  </si>
+  <si>
+    <t>Ondas y Electromagnetismo</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>No presencial</t>
+  </si>
+  <si>
+    <t>13:15:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-008</t>
+  </si>
+  <si>
+    <t>BBDD</t>
+  </si>
+  <si>
+    <t>Bases de Datos</t>
+  </si>
+  <si>
+    <t>18:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-010</t>
+  </si>
+  <si>
+    <t>IAE</t>
+  </si>
+  <si>
+    <t>Integración de aplicaciones empresariales</t>
+  </si>
+  <si>
+    <t>18:15:00</t>
+  </si>
+  <si>
+    <t>19:15:00</t>
+  </si>
+  <si>
     <t>GIISOF01-2-002</t>
   </si>
   <si>
@@ -71,160 +203,430 @@
     <t>Arquitectura de Computadores</t>
   </si>
   <si>
-    <t>Teórico</t>
-  </si>
-  <si>
-    <t>Presencial</t>
-  </si>
-  <si>
     <t>2:30:00</t>
   </si>
   <si>
-    <t>lunes</t>
-  </si>
-  <si>
-    <t>9:00:00</t>
+    <t>miércoles</t>
   </si>
   <si>
     <t>11:30:00</t>
   </si>
   <si>
+    <t>GIISOF01-1-010</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Metodología de la Programación</t>
+  </si>
+  <si>
+    <t>11:45:00</t>
+  </si>
+  <si>
+    <t>14:45:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-006</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>Administración de Sistemas y Redes</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-003</t>
+  </si>
+  <si>
+    <t>CVVS</t>
+  </si>
+  <si>
+    <t>Calidad, Validación y Verificación del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-017</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>Software para Robots</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>9:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-002 </t>
+  </si>
+  <si>
+    <t>SEW</t>
+  </si>
+  <si>
+    <t>Software y Estándares para la Web</t>
+  </si>
+  <si>
+    <t>Presentación</t>
+  </si>
+  <si>
+    <t>9:45:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-004</t>
+  </si>
+  <si>
+    <t>DPPI</t>
+  </si>
+  <si>
+    <t>Dirección y Planificación de Proyectos Informáticos</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-009 </t>
+  </si>
+  <si>
+    <t>Computación Numérica</t>
+  </si>
+  <si>
+    <t>17:45:00</t>
+  </si>
+  <si>
+    <t>20:45:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-003</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Estructura de Datos</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-003</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>Ingeniería del Proceso Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-001</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática (80)</t>
+  </si>
+  <si>
+    <t>2:00:00</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-008</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Sistemas Inteligentes</t>
+  </si>
+  <si>
+    <t>17:15:00</t>
+  </si>
+  <si>
+    <t>19:45:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-009 </t>
+  </si>
+  <si>
+    <t>DLP</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
+  </si>
+  <si>
+    <t>3:30:00</t>
+  </si>
+  <si>
+    <t>12:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-002</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Ingeniería de Requisitos</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-007</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Introducción a la Programación</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>18:30:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-001</t>
+  </si>
+  <si>
+    <t>TEC</t>
+  </si>
+  <si>
+    <t>Tecnología Electrónica de Computadores</t>
+  </si>
+  <si>
+    <t>18:45:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-007</t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>Comunicación Persona-Máquina</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-016</t>
+  </si>
+  <si>
+    <t>SEV</t>
+  </si>
+  <si>
+    <t>Software de entretenimiento y videojuegos</t>
+  </si>
+  <si>
+    <t>10:15:00</t>
+  </si>
+  <si>
+    <t>10:45:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-002</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Álgebra Lineal</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-011</t>
+  </si>
+  <si>
+    <t>IFA</t>
+  </si>
+  <si>
+    <t>Informática Forense y Auditoría</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-004</t>
+  </si>
+  <si>
+    <t>TPP</t>
+  </si>
+  <si>
+    <t>Tecnología y Paradigmas de Programación</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-009</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>Autómatas y Matemáticas Discretas</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-004</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Diseño del Software</t>
+  </si>
+  <si>
+    <t>GIISOF01-3-002</t>
+  </si>
+  <si>
+    <t>1:30:00</t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-005 </t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>Sistemas Distribuidos e Internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-0-013 </t>
+  </si>
+  <si>
+    <t>SDM</t>
+  </si>
+  <si>
+    <t>Software para Dispositivos Móviles</t>
+  </si>
+  <si>
+    <t>15:15:00</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-004 </t>
+  </si>
+  <si>
+    <t>GIISOF01-0-018</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Informática Audiovisual</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-004</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Cálculo</t>
+  </si>
+  <si>
+    <t>16:15:00</t>
+  </si>
+  <si>
+    <t>11:15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-010 </t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Seguridad de Sistemas Informáticos</t>
+  </si>
+  <si>
+    <t>GIISOF01-4-005</t>
+  </si>
+  <si>
+    <t>ASLEPI</t>
+  </si>
+  <si>
+    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
+  </si>
+  <si>
+    <t>GIISOF01-1-003</t>
+  </si>
+  <si>
+    <t>Emp</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-3-008 </t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Arquitectura del Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-001 </t>
+  </si>
+  <si>
+    <t>GIISOF01-1-006</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Estadística</t>
+  </si>
+  <si>
+    <t>GIISOF01-0-013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-007 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIISOF01-2-010 </t>
+  </si>
+  <si>
+    <t>Alg</t>
+  </si>
+  <si>
+    <t>Algoritmia</t>
+  </si>
+  <si>
+    <t>13:45:00</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>GIISOF01-3-010</t>
+  </si>
+  <si>
+    <t>GIISOF01-2-010</t>
+  </si>
+  <si>
+    <t>Fundamentos de Informática</t>
+  </si>
+  <si>
+    <t>14:15:00</t>
+  </si>
+  <si>
     <t>GIISOF01-3-008</t>
   </si>
   <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>No presencial</t>
-  </si>
-  <si>
-    <t>1:00:00</t>
-  </si>
-  <si>
-    <t>12:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-013 </t>
-  </si>
-  <si>
-    <t>SDM</t>
-  </si>
-  <si>
-    <t>Software para Dispositivos Móviles</t>
-  </si>
-  <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
-    <t>Entrega</t>
-  </si>
-  <si>
-    <t>0:30:00</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-001</t>
-  </si>
-  <si>
-    <t>FI</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática</t>
-  </si>
-  <si>
-    <t>2:00:00</t>
-  </si>
-  <si>
-    <t>15:00:00</t>
-  </si>
-  <si>
-    <t>17:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-005</t>
-  </si>
-  <si>
-    <t>ASLEPI</t>
-  </si>
-  <si>
-    <t>Aspectos Sociales, Legales, Éticos y Prof. de la Informática</t>
-  </si>
-  <si>
-    <t>martes</t>
-  </si>
-  <si>
-    <t>10:00:00</t>
-  </si>
-  <si>
-    <t>Fundamentos de Informática (80)</t>
-  </si>
-  <si>
-    <t>Práctico</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-010</t>
-  </si>
-  <si>
-    <t>SSI</t>
-  </si>
-  <si>
-    <t>Seguridad de Sistemas Informáticos</t>
-  </si>
-  <si>
-    <t>1:30:00</t>
-  </si>
-  <si>
-    <t>13:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-008</t>
-  </si>
-  <si>
-    <t>BBDD</t>
-  </si>
-  <si>
-    <t>Bases de Datos</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-008 </t>
-  </si>
-  <si>
-    <t>Presentación</t>
-  </si>
-  <si>
-    <t>miércoles</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-008</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Sistemas Inteligentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-0-015 </t>
-  </si>
-  <si>
-    <t>SIW</t>
-  </si>
-  <si>
-    <t>Sistemas de Información para la Web</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
+    <t>GIISOF01-3-005</t>
   </si>
   <si>
     <t>GIISOF01-2-005</t>
@@ -234,363 +636,6 @@
   </si>
   <si>
     <t>Computabilidad</t>
-  </si>
-  <si>
-    <t>3:00:00</t>
-  </si>
-  <si>
-    <t>18:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-008</t>
-  </si>
-  <si>
-    <t>FCR</t>
-  </si>
-  <si>
-    <t>Fundamentos de Computadores y Redes</t>
-  </si>
-  <si>
-    <t>jueves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-009 </t>
-  </si>
-  <si>
-    <t>DLP</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 2)</t>
-  </si>
-  <si>
-    <t>3:30:00</t>
-  </si>
-  <si>
-    <t>15:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-006</t>
-  </si>
-  <si>
-    <t>SSOO</t>
-  </si>
-  <si>
-    <t>Sistemas Operativos</t>
-  </si>
-  <si>
-    <t>18:30:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-005 </t>
-  </si>
-  <si>
-    <t>SDI</t>
-  </si>
-  <si>
-    <t>Sistemas Distribuidos e Internet</t>
-  </si>
-  <si>
-    <t>20:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-003</t>
-  </si>
-  <si>
-    <t>Emp</t>
-  </si>
-  <si>
-    <t>Empresa</t>
-  </si>
-  <si>
-    <t>viernes</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-001</t>
-  </si>
-  <si>
-    <t>RI</t>
-  </si>
-  <si>
-    <t>Repositorios de Información</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-013</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-009</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>Autómatas y Matemáticas Discretas</t>
-  </si>
-  <si>
-    <t>11:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-009</t>
-  </si>
-  <si>
-    <t>Computación Numérica</t>
-  </si>
-  <si>
-    <t>14:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-017</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>Software para Robots</t>
-  </si>
-  <si>
-    <t>Diseño de Lenguajes de Programación 100 (tanda 1)</t>
-  </si>
-  <si>
-    <t>19:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-010</t>
-  </si>
-  <si>
-    <t>Alg</t>
-  </si>
-  <si>
-    <t>Algoritmia</t>
-  </si>
-  <si>
-    <t>GIISOF01-4-002</t>
-  </si>
-  <si>
-    <t>IR</t>
-  </si>
-  <si>
-    <t>Ingeniería de Requisitos</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-010</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>Metodología de la Programación</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-002</t>
-  </si>
-  <si>
-    <t>SEW</t>
-  </si>
-  <si>
-    <t>Software y Estándares para la Web</t>
-  </si>
-  <si>
-    <t>19:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-010</t>
-  </si>
-  <si>
-    <t>IAE</t>
-  </si>
-  <si>
-    <t>Integración de aplicaciones empresariales</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-004</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>Diseño del Software</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-005</t>
-  </si>
-  <si>
-    <t>OyE</t>
-  </si>
-  <si>
-    <t>Ondas y Electromagnetismo</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-003</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>Estructura de Datos</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-018</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>Informática Audiovisual</t>
-  </si>
-  <si>
-    <t>9:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-003</t>
-  </si>
-  <si>
-    <t>IPS</t>
-  </si>
-  <si>
-    <t>Ingeniería del Proceso Software</t>
-  </si>
-  <si>
-    <t>10:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-1-007</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Introducción a la Programación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-010 </t>
-  </si>
-  <si>
-    <t>GIISOF01-1-002</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>Álgebra Lineal</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-016</t>
-  </si>
-  <si>
-    <t>SEV</t>
-  </si>
-  <si>
-    <t>Software de entretenimiento y videojuegos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-001 </t>
-  </si>
-  <si>
-    <t>TEC</t>
-  </si>
-  <si>
-    <t>Tecnología Electrónica de Computadores</t>
-  </si>
-  <si>
-    <t>16:30:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-004</t>
-  </si>
-  <si>
-    <t>TPP</t>
-  </si>
-  <si>
-    <t>Tecnología y Paradigmas de Programación</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-007</t>
-  </si>
-  <si>
-    <t>CPM</t>
-  </si>
-  <si>
-    <t>Comunicación Persona-Máquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-004 </t>
-  </si>
-  <si>
-    <t>GIISOF01-4-003</t>
-  </si>
-  <si>
-    <t>CVVS</t>
-  </si>
-  <si>
-    <t>Calidad, Validación y Verificación del Software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-007 </t>
-  </si>
-  <si>
-    <t>GIISOF01-1-004</t>
-  </si>
-  <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Cálculo</t>
-  </si>
-  <si>
-    <t>GIISOF01-0-011</t>
-  </si>
-  <si>
-    <t>IFA</t>
-  </si>
-  <si>
-    <t>Informática Forense y Auditoría</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-006</t>
-  </si>
-  <si>
-    <t>ASR</t>
-  </si>
-  <si>
-    <t>Administración de Sistemas y Redes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-009 </t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-2-010 </t>
-  </si>
-  <si>
-    <t>GIISOF01-1-006</t>
-  </si>
-  <si>
-    <t>Est</t>
-  </si>
-  <si>
-    <t>Estadística</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIISOF01-3-002 </t>
-  </si>
-  <si>
-    <t>GIISOF01-4-004</t>
-  </si>
-  <si>
-    <t>DPPI</t>
-  </si>
-  <si>
-    <t>Dirección y Planificación de Proyectos Informáticos</t>
-  </si>
-  <si>
-    <t>GIISOF01-3-005</t>
-  </si>
-  <si>
-    <t>GIISOF01-2-001</t>
   </si>
 </sst>
 </file>
@@ -693,10 +738,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -708,7 +753,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -717,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="n">
-        <v>60.0</v>
+        <v>20.0</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -738,15 +783,15 @@
         <v>1.0</v>
       </c>
       <c r="P2" t="n">
-        <v>4.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -758,19 +803,19 @@
         <v>27</v>
       </c>
       <c r="F3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" t="n">
         <v>0.0</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K3" t="n">
         <v>44361.0</v>
@@ -779,48 +824,48 @@
         <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O3" t="n">
         <v>1.0</v>
       </c>
       <c r="P3" t="n">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.0</v>
       </c>
-      <c r="B4" t="n">
-        <v>1.0</v>
-      </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I4" t="n">
         <v>0.0</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K4" t="n">
         <v>44361.0</v>
@@ -829,7 +874,7 @@
         <v>22</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N4" t="s">
         <v>37</v>
@@ -838,15 +883,15 @@
         <v>1.0</v>
       </c>
       <c r="P4" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -861,16 +906,16 @@
         <v>1.0</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="n">
-        <v>80.0</v>
+        <v>40.0</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" t="n">
         <v>44361.0</v>
@@ -879,283 +924,283 @@
         <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O5" t="n">
         <v>1.0</v>
       </c>
       <c r="P5" t="n">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="B6" t="n">
         <v>2.0</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" t="n">
         <v>1.0</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I6" t="n">
-        <v>177.0</v>
+        <v>150.0</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K6" t="n">
         <v>44362.0</v>
       </c>
       <c r="L6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M6" t="s">
         <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="O6" t="n">
         <v>1.0</v>
       </c>
       <c r="P6" t="n">
-        <v>53.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B7" t="n">
         <v>1.0</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="F7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
       <c r="I7" t="n">
-        <v>79.0</v>
+        <v>67.0</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K7" t="n">
         <v>44362.0</v>
       </c>
       <c r="L7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="N7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O7" t="n">
         <v>1.0</v>
       </c>
       <c r="P7" t="n">
-        <v>29.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B8" t="n">
         <v>2.0</v>
       </c>
       <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
       <c r="F8" t="n">
         <v>1.0</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="n">
-        <v>116.0</v>
+        <v>60.0</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="K8" t="n">
         <v>44362.0</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M8" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="N8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O8" t="n">
         <v>1.0</v>
       </c>
       <c r="P8" t="n">
-        <v>27.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B9" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>59</v>
-      </c>
       <c r="F9" t="n">
         <v>1.0</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I9" t="n">
-        <v>71.0</v>
+        <v>3.0</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="K9" t="n">
         <v>44362.0</v>
       </c>
       <c r="L9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O9" t="n">
         <v>1.0</v>
       </c>
       <c r="P9" t="n">
-        <v>55.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B10" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
         <v>61</v>
       </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="F10" t="n">
         <v>2.0</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0</v>
+        <v>60.0</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="K10" t="n">
         <v>44363.0</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M10" t="s">
         <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="O10" t="n">
         <v>1.0</v>
       </c>
       <c r="P10" t="n">
-        <v>22.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F11" t="n">
         <v>1.0</v>
@@ -1167,7 +1212,7 @@
         <v>20</v>
       </c>
       <c r="I11" t="n">
-        <v>103.0</v>
+        <v>50.0</v>
       </c>
       <c r="J11" t="s">
         <v>21</v>
@@ -1176,169 +1221,169 @@
         <v>44363.0</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M11" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="N11" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="O11" t="n">
         <v>1.0</v>
       </c>
       <c r="P11" t="n">
-        <v>6.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F12" t="n">
         <v>1.0</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I12" t="n">
         <v>0.0</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K12" t="n">
         <v>44363.0</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="O12" t="n">
         <v>1.0</v>
       </c>
       <c r="P12" t="n">
-        <v>19.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B13" t="n">
         <v>1.0</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F13" t="n">
         <v>1.0</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
       </c>
       <c r="I13" t="n">
-        <v>70.0</v>
+        <v>45.0</v>
       </c>
       <c r="J13" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="K13" t="n">
         <v>44363.0</v>
       </c>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N13" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="O13" t="n">
         <v>1.0</v>
       </c>
       <c r="P13" t="n">
-        <v>52.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B14" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F14" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I14" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="J14" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="K14" t="n">
         <v>44364.0</v>
       </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M14" t="s">
         <v>23</v>
       </c>
       <c r="N14" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="O14" t="n">
         <v>1.0</v>
       </c>
       <c r="P14" t="n">
-        <v>61.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="15">
@@ -1346,166 +1391,166 @@
         <v>3.0</v>
       </c>
       <c r="B15" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F15" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="I15" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="K15" t="n">
         <v>44364.0</v>
       </c>
       <c r="L15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M15" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="N15" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="O15" t="n">
         <v>1.0</v>
       </c>
       <c r="P15" t="n">
-        <v>60.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B16" t="n">
         <v>2.0</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F16" t="n">
         <v>1.0</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I16" t="n">
-        <v>40.0</v>
+        <v>120.0</v>
       </c>
       <c r="J16" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K16" t="n">
         <v>44364.0</v>
       </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M16" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="N16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="O16" t="n">
         <v>1.0</v>
       </c>
       <c r="P16" t="n">
-        <v>31.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B17" t="n">
         <v>2.0</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" t="n">
         <v>2.0</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="J17" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="K17" t="n">
         <v>44364.0</v>
       </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M17" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O17" t="n">
         <v>1.0</v>
       </c>
       <c r="P17" t="n">
-        <v>48.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B18" t="n">
         <v>1.0</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F18" t="n">
         <v>1.0</v>
@@ -1517,7 +1562,7 @@
         <v>20</v>
       </c>
       <c r="I18" t="n">
-        <v>44.0</v>
+        <v>62.0</v>
       </c>
       <c r="J18" t="s">
         <v>21</v>
@@ -1526,7 +1571,7 @@
         <v>44365.0</v>
       </c>
       <c r="L18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M18" t="s">
         <v>23</v>
@@ -1538,30 +1583,30 @@
         <v>1.0</v>
       </c>
       <c r="P18" t="n">
-        <v>38.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="F19" t="n">
         <v>1.0</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H19" t="s">
         <v>20</v>
@@ -1570,157 +1615,157 @@
         <v>40.0</v>
       </c>
       <c r="J19" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="K19" t="n">
         <v>44365.0</v>
       </c>
       <c r="L19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N19" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O19" t="n">
         <v>1.0</v>
       </c>
       <c r="P19" t="n">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F20" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0</v>
+        <v>79.0</v>
       </c>
       <c r="J20" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="K20" t="n">
         <v>44365.0</v>
       </c>
       <c r="L20" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M20" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="O20" t="n">
         <v>1.0</v>
       </c>
       <c r="P20" t="n">
-        <v>0.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="B21" t="n">
         <v>1.0</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="F21" t="n">
         <v>1.0</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0</v>
+        <v>103.0</v>
       </c>
       <c r="J21" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="K21" t="n">
         <v>44365.0</v>
       </c>
       <c r="L21" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M21" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="N21" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="O21" t="n">
         <v>1.0</v>
       </c>
       <c r="P21" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B22" t="n">
         <v>2.0</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="F22" t="n">
         <v>2.0</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H22" t="s">
         <v>20</v>
       </c>
       <c r="I22" t="n">
-        <v>70.0</v>
+        <v>89.0</v>
       </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="K22" t="n">
         <v>44368.0</v>
@@ -1732,45 +1777,45 @@
         <v>23</v>
       </c>
       <c r="N22" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="O22" t="n">
         <v>1.0</v>
       </c>
       <c r="P22" t="n">
-        <v>32.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B23" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="F23" t="n">
         <v>1.0</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H23" t="s">
         <v>20</v>
       </c>
       <c r="I23" t="n">
-        <v>50.0</v>
+        <v>90.0</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K23" t="n">
         <v>44368.0</v>
@@ -1779,48 +1824,48 @@
         <v>22</v>
       </c>
       <c r="M23" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="N23" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="O23" t="n">
         <v>1.0</v>
       </c>
       <c r="P23" t="n">
-        <v>18.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B24" t="n">
         <v>1.0</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="J24" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="K24" t="n">
         <v>44368.0</v>
@@ -1829,48 +1874,48 @@
         <v>22</v>
       </c>
       <c r="M24" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="N24" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="O24" t="n">
         <v>1.0</v>
       </c>
       <c r="P24" t="n">
-        <v>50.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I25" t="n">
-        <v>89.0</v>
+        <v>8.0</v>
       </c>
       <c r="J25" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="K25" t="n">
         <v>44368.0</v>
@@ -1879,16 +1924,16 @@
         <v>22</v>
       </c>
       <c r="M25" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="N25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O25" t="n">
         <v>1.0</v>
       </c>
       <c r="P25" t="n">
-        <v>58.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="26">
@@ -1896,99 +1941,99 @@
         <v>2.0</v>
       </c>
       <c r="B26" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="E26" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F26" t="n">
         <v>1.0</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I26" t="n">
-        <v>100.0</v>
+        <v>84.0</v>
       </c>
       <c r="J26" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="K26" t="n">
         <v>44369.0</v>
       </c>
       <c r="L26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M26" t="s">
         <v>23</v>
       </c>
       <c r="N26" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="O26" t="n">
         <v>1.0</v>
       </c>
       <c r="P26" t="n">
-        <v>24.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="B27" t="n">
         <v>1.0</v>
       </c>
       <c r="C27" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="E27" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="F27" t="n">
         <v>1.0</v>
       </c>
       <c r="G27" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I27" t="n">
-        <v>90.0</v>
+        <v>0.0</v>
       </c>
       <c r="J27" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="K27" t="n">
         <v>44369.0</v>
       </c>
       <c r="L27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M27" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="N27" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="O27" t="n">
         <v>1.0</v>
       </c>
       <c r="P27" t="n">
-        <v>10.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="28">
@@ -1996,49 +2041,49 @@
         <v>1.0</v>
       </c>
       <c r="B28" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="F28" t="n">
         <v>1.0</v>
       </c>
       <c r="G28" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H28" t="s">
         <v>20</v>
       </c>
       <c r="I28" t="n">
-        <v>50.0</v>
+        <v>120.0</v>
       </c>
       <c r="J28" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K28" t="n">
         <v>44369.0</v>
       </c>
       <c r="L28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M28" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
       <c r="N28" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="O28" t="n">
         <v>1.0</v>
       </c>
       <c r="P28" t="n">
-        <v>17.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="29">
@@ -2046,49 +2091,49 @@
         <v>3.0</v>
       </c>
       <c r="B29" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="F29" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G29" t="s">
         <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I29" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="J29" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="K29" t="n">
         <v>44369.0</v>
       </c>
       <c r="L29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M29" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="N29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O29" t="n">
         <v>1.0</v>
       </c>
       <c r="P29" t="n">
-        <v>33.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="30">
@@ -2099,63 +2144,63 @@
         <v>1.0</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="F30" t="n">
         <v>1.0</v>
       </c>
       <c r="G30" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H30" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="I30" t="n">
         <v>3.0</v>
       </c>
       <c r="J30" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="K30" t="n">
         <v>44370.0</v>
       </c>
       <c r="L30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M30" t="s">
         <v>23</v>
       </c>
       <c r="N30" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="O30" t="n">
         <v>1.0</v>
       </c>
       <c r="P30" t="n">
-        <v>25.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B31" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C31" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="E31" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="F31" t="n">
         <v>1.0</v>
@@ -2167,28 +2212,28 @@
         <v>20</v>
       </c>
       <c r="I31" t="n">
-        <v>150.0</v>
+        <v>61.0</v>
       </c>
       <c r="J31" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="K31" t="n">
         <v>44370.0</v>
       </c>
       <c r="L31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M31" t="s">
-        <v>48</v>
+        <v>136</v>
       </c>
       <c r="N31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O31" t="n">
         <v>1.0</v>
       </c>
       <c r="P31" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="32">
@@ -2199,16 +2244,16 @@
         <v>2.0</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F32" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G32" t="s">
         <v>19</v>
@@ -2217,128 +2262,128 @@
         <v>20</v>
       </c>
       <c r="I32" t="n">
-        <v>150.0</v>
+        <v>70.0</v>
       </c>
       <c r="J32" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="K32" t="n">
         <v>44370.0</v>
       </c>
       <c r="L32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M32" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N32" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="O32" t="n">
         <v>1.0</v>
       </c>
       <c r="P32" t="n">
-        <v>26.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B33" t="n">
         <v>1.0</v>
       </c>
       <c r="C33" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="D33" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="E33" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="F33" t="n">
         <v>1.0</v>
       </c>
       <c r="G33" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H33" t="s">
         <v>20</v>
       </c>
       <c r="I33" t="n">
-        <v>62.0</v>
+        <v>150.0</v>
       </c>
       <c r="J33" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K33" t="n">
         <v>44370.0</v>
       </c>
       <c r="L33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M33" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="N33" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="O33" t="n">
         <v>1.0</v>
       </c>
       <c r="P33" t="n">
-        <v>35.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="B34" t="n">
         <v>1.0</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="F34" t="n">
         <v>1.0</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H34" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I34" t="n">
         <v>0.0</v>
       </c>
       <c r="J34" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="K34" t="n">
         <v>44371.0</v>
       </c>
       <c r="L34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M34" t="s">
         <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="O34" t="n">
         <v>1.0</v>
       </c>
       <c r="P34" t="n">
-        <v>36.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="35">
@@ -2346,140 +2391,140 @@
         <v>3.0</v>
       </c>
       <c r="B35" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C35" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="E35" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="F35" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G35" t="s">
         <v>19</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I35" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="J35" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="K35" t="n">
         <v>44371.0</v>
       </c>
       <c r="L35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="N35" t="s">
-        <v>145</v>
+        <v>31</v>
       </c>
       <c r="O35" t="n">
         <v>1.0</v>
       </c>
       <c r="P35" t="n">
-        <v>11.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B36" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>52</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="F36" t="n">
         <v>1.0</v>
       </c>
       <c r="G36" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H36" t="s">
         <v>20</v>
       </c>
       <c r="I36" t="n">
-        <v>50.0</v>
+        <v>71.0</v>
       </c>
       <c r="J36" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="K36" t="n">
         <v>44371.0</v>
       </c>
       <c r="L36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M36" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="N36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O36" t="n">
         <v>1.0</v>
       </c>
       <c r="P36" t="n">
-        <v>44.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="B37" t="n">
         <v>1.0</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="F37" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G37" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H37" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I37" t="n">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="J37" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K37" t="n">
         <v>44371.0</v>
       </c>
       <c r="L37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M37" t="s">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="N37" t="s">
         <v>43</v>
@@ -2488,36 +2533,36 @@
         <v>1.0</v>
       </c>
       <c r="P37" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B38" t="n">
         <v>2.0</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="F38" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G38" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H38" t="s">
         <v>20</v>
       </c>
       <c r="I38" t="n">
-        <v>71.0</v>
+        <v>50.0</v>
       </c>
       <c r="J38" t="s">
         <v>21</v>
@@ -2526,7 +2571,7 @@
         <v>44372.0</v>
       </c>
       <c r="L38" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M38" t="s">
         <v>23</v>
@@ -2538,27 +2583,27 @@
         <v>1.0</v>
       </c>
       <c r="P38" t="n">
-        <v>51.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B39" t="n">
         <v>1.0</v>
       </c>
       <c r="C39" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="D39" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F39" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G39" t="s">
         <v>19</v>
@@ -2567,28 +2612,28 @@
         <v>20</v>
       </c>
       <c r="I39" t="n">
-        <v>120.0</v>
+        <v>79.0</v>
       </c>
       <c r="J39" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K39" t="n">
         <v>44372.0</v>
       </c>
       <c r="L39" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M39" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N39" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
       <c r="O39" t="n">
         <v>1.0</v>
       </c>
       <c r="P39" t="n">
-        <v>56.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="40">
@@ -2599,96 +2644,96 @@
         <v>1.0</v>
       </c>
       <c r="C40" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="E40" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="F40" t="n">
         <v>1.0</v>
       </c>
       <c r="G40" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H40" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I40" t="n">
         <v>0.0</v>
       </c>
       <c r="J40" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K40" t="n">
         <v>44372.0</v>
       </c>
       <c r="L40" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M40" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N40" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="O40" t="n">
         <v>1.0</v>
       </c>
       <c r="P40" t="n">
-        <v>54.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B41" t="n">
         <v>1.0</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="E41" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="F41" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G41" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H41" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I41" t="n">
-        <v>8.0</v>
+        <v>140.0</v>
       </c>
       <c r="J41" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K41" t="n">
         <v>44372.0</v>
       </c>
       <c r="L41" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M41" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="N41" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="O41" t="n">
         <v>1.0</v>
       </c>
       <c r="P41" t="n">
-        <v>59.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="42">
@@ -2696,31 +2741,31 @@
         <v>2.0</v>
       </c>
       <c r="B42" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C42" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="D42" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
       <c r="F42" t="n">
         <v>1.0</v>
       </c>
       <c r="G42" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H42" t="s">
         <v>20</v>
       </c>
       <c r="I42" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="J42" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="K42" t="n">
         <v>44375.0</v>
@@ -2732,45 +2777,45 @@
         <v>23</v>
       </c>
       <c r="N42" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="O42" t="n">
         <v>1.0</v>
       </c>
       <c r="P42" t="n">
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="B43" t="n">
         <v>1.0</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="F43" t="n">
         <v>1.0</v>
       </c>
       <c r="G43" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H43" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="I43" t="n">
-        <v>67.0</v>
+        <v>0.0</v>
       </c>
       <c r="J43" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="K43" t="n">
         <v>44375.0</v>
@@ -2779,48 +2824,48 @@
         <v>22</v>
       </c>
       <c r="M43" t="s">
-        <v>24</v>
+        <v>175</v>
       </c>
       <c r="N43" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="O43" t="n">
         <v>1.0</v>
       </c>
       <c r="P43" t="n">
-        <v>9.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B44" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E44" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="F44" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G44" t="s">
         <v>19</v>
       </c>
       <c r="H44" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I44" t="n">
-        <v>84.0</v>
+        <v>71.0</v>
       </c>
       <c r="J44" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="K44" t="n">
         <v>44375.0</v>
@@ -2829,48 +2874,48 @@
         <v>22</v>
       </c>
       <c r="M44" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N44" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="O44" t="n">
         <v>1.0</v>
       </c>
       <c r="P44" t="n">
-        <v>16.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="B45" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>179</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>180</v>
       </c>
       <c r="E45" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
       <c r="F45" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G45" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H45" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0</v>
+        <v>177.0</v>
       </c>
       <c r="J45" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="K45" t="n">
         <v>44375.0</v>
@@ -2879,116 +2924,116 @@
         <v>22</v>
       </c>
       <c r="M45" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="N45" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="O45" t="n">
         <v>1.0</v>
       </c>
       <c r="P45" t="n">
-        <v>20.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B46" t="n">
         <v>1.0</v>
       </c>
       <c r="C46" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="E46" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="F46" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G46" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H46" t="s">
         <v>20</v>
       </c>
       <c r="I46" t="n">
-        <v>79.0</v>
+        <v>44.0</v>
       </c>
       <c r="J46" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K46" t="n">
         <v>44376.0</v>
       </c>
       <c r="L46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M46" t="s">
         <v>23</v>
       </c>
       <c r="N46" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="O46" t="n">
         <v>1.0</v>
       </c>
       <c r="P46" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B47" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="D47" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="E47" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="F47" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G47" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H47" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="I47" t="n">
-        <v>45.0</v>
+        <v>0.0</v>
       </c>
       <c r="J47" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="K47" t="n">
         <v>44376.0</v>
       </c>
       <c r="L47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M47" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="N47" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="O47" t="n">
         <v>1.0</v>
       </c>
       <c r="P47" t="n">
-        <v>30.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="48">
@@ -2999,75 +3044,75 @@
         <v>1.0</v>
       </c>
       <c r="C48" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="D48" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="E48" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="F48" t="n">
         <v>2.0</v>
       </c>
       <c r="G48" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H48" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="I48" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="J48" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="K48" t="n">
         <v>44376.0</v>
       </c>
       <c r="L48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M48" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="N48" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="O48" t="n">
         <v>1.0</v>
       </c>
       <c r="P48" t="n">
-        <v>42.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B49" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="E49" t="s">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="F49" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G49" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H49" t="s">
         <v>20</v>
       </c>
       <c r="I49" t="n">
-        <v>60.0</v>
+        <v>183.0</v>
       </c>
       <c r="J49" t="s">
         <v>21</v>
@@ -3076,7 +3121,7 @@
         <v>44377.0</v>
       </c>
       <c r="L49" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M49" t="s">
         <v>23</v>
@@ -3088,145 +3133,145 @@
         <v>1.0</v>
       </c>
       <c r="P49" t="n">
-        <v>28.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B50" t="n">
         <v>1.0</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="D50" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E50" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="F50" t="n">
         <v>1.0</v>
       </c>
       <c r="G50" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H50" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I50" t="n">
-        <v>140.0</v>
+        <v>0.0</v>
       </c>
       <c r="J50" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="K50" t="n">
         <v>44377.0</v>
       </c>
       <c r="L50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M50" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N50" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="O50" t="n">
         <v>1.0</v>
       </c>
       <c r="P50" t="n">
-        <v>40.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="B51" t="n">
         <v>1.0</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="D51" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="E51" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="F51" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G51" t="s">
         <v>19</v>
       </c>
       <c r="H51" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="I51" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="J51" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K51" t="n">
         <v>44377.0</v>
       </c>
       <c r="L51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M51" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="N51" t="s">
-        <v>177</v>
+        <v>54</v>
       </c>
       <c r="O51" t="n">
         <v>1.0</v>
       </c>
       <c r="P51" t="n">
-        <v>41.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B52" t="n">
         <v>2.0</v>
       </c>
       <c r="C52" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="D52" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="E52" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F52" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G52" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H52" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I52" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="J52" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="K52" t="n">
         <v>44378.0</v>
       </c>
       <c r="L52" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M52" t="s">
         <v>23</v>
@@ -3238,7 +3283,7 @@
         <v>1.0</v>
       </c>
       <c r="P52" t="n">
-        <v>5.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="53">
@@ -3246,266 +3291,266 @@
         <v>2.0</v>
       </c>
       <c r="B53" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C53" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="F53" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G53" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H53" t="s">
         <v>20</v>
       </c>
       <c r="I53" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c r="J53" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K53" t="n">
         <v>44378.0</v>
       </c>
       <c r="L53" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M53" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="N53" t="s">
-        <v>30</v>
+        <v>197</v>
       </c>
       <c r="O53" t="n">
         <v>1.0</v>
       </c>
       <c r="P53" t="n">
-        <v>49.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B54" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E54" t="s">
-        <v>182</v>
+        <v>84</v>
       </c>
       <c r="F54" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G54" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H54" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I54" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="J54" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K54" t="n">
         <v>44378.0</v>
       </c>
       <c r="L54" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M54" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N54" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="O54" t="n">
         <v>1.0</v>
       </c>
       <c r="P54" t="n">
-        <v>14.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B55" t="n">
         <v>2.0</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="D55" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="E55" t="s">
-        <v>115</v>
+        <v>198</v>
       </c>
       <c r="F55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G55" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H55" t="s">
         <v>20</v>
       </c>
       <c r="I55" t="n">
-        <v>30.0</v>
+        <v>70.0</v>
       </c>
       <c r="J55" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="K55" t="n">
         <v>44379.0</v>
       </c>
       <c r="L55" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M55" t="s">
         <v>23</v>
       </c>
       <c r="N55" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="O55" t="n">
         <v>1.0</v>
       </c>
       <c r="P55" t="n">
-        <v>46.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B56" t="n">
         <v>2.0</v>
       </c>
       <c r="C56" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="D56" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E56" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F56" t="n">
         <v>1.0</v>
       </c>
       <c r="G56" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H56" t="s">
         <v>20</v>
       </c>
       <c r="I56" t="n">
-        <v>183.0</v>
+        <v>116.0</v>
       </c>
       <c r="J56" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="K56" t="n">
         <v>44379.0</v>
       </c>
       <c r="L56" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M56" t="s">
-        <v>104</v>
+        <v>175</v>
       </c>
       <c r="N56" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="O56" t="n">
         <v>1.0</v>
       </c>
       <c r="P56" t="n">
-        <v>47.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B57" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C57" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="D57" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="E57" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
       <c r="F57" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G57" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H57" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I57" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="J57" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="K57" t="n">
         <v>44379.0</v>
       </c>
       <c r="L57" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M57" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="N57" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="O57" t="n">
         <v>1.0</v>
       </c>
       <c r="P57" t="n">
-        <v>34.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B58" t="n">
         <v>2.0</v>
       </c>
       <c r="C58" t="s">
-        <v>188</v>
+        <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>189</v>
+        <v>39</v>
       </c>
       <c r="E58" t="s">
-        <v>190</v>
+        <v>40</v>
       </c>
       <c r="F58" t="n">
         <v>1.0</v>
@@ -3514,10 +3559,10 @@
         <v>19</v>
       </c>
       <c r="H58" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I58" t="n">
-        <v>120.0</v>
+        <v>40.0</v>
       </c>
       <c r="J58" t="s">
         <v>21</v>
@@ -3538,39 +3583,39 @@
         <v>1.0</v>
       </c>
       <c r="P58" t="n">
-        <v>45.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B59" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C59" t="s">
-        <v>191</v>
+        <v>102</v>
       </c>
       <c r="D59" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E59" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="F59" t="n">
         <v>1.0</v>
       </c>
       <c r="G59" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H59" t="s">
         <v>20</v>
       </c>
       <c r="I59" t="n">
-        <v>40.0</v>
+        <v>80.0</v>
       </c>
       <c r="J59" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="K59" t="n">
         <v>44382.0</v>
@@ -3579,48 +3624,48 @@
         <v>22</v>
       </c>
       <c r="M59" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="N59" t="s">
-        <v>56</v>
+        <v>202</v>
       </c>
       <c r="O59" t="n">
         <v>1.0</v>
       </c>
       <c r="P59" t="n">
-        <v>15.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B60" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C60" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="D60" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="E60" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="F60" t="n">
         <v>1.0</v>
       </c>
       <c r="G60" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H60" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="I60" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="J60" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="K60" t="n">
         <v>44382.0</v>
@@ -3629,66 +3674,66 @@
         <v>22</v>
       </c>
       <c r="M60" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="N60" t="s">
-        <v>177</v>
+        <v>123</v>
       </c>
       <c r="O60" t="n">
         <v>1.0</v>
       </c>
       <c r="P60" t="n">
-        <v>57.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B61" t="n">
         <v>2.0</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>204</v>
       </c>
       <c r="D61" t="s">
-        <v>77</v>
+        <v>160</v>
       </c>
       <c r="E61" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="F61" t="n">
         <v>1.0</v>
       </c>
       <c r="G61" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H61" t="s">
         <v>20</v>
       </c>
       <c r="I61" t="n">
-        <v>0.0</v>
+        <v>40.0</v>
       </c>
       <c r="J61" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="K61" t="n">
         <v>44383.0</v>
       </c>
       <c r="L61" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M61" t="s">
         <v>23</v>
       </c>
       <c r="N61" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="O61" t="n">
         <v>1.0</v>
       </c>
       <c r="P61" t="n">
-        <v>23.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="62">
@@ -3696,99 +3741,99 @@
         <v>2.0</v>
       </c>
       <c r="B62" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>205</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>206</v>
       </c>
       <c r="E62" t="s">
-        <v>59</v>
+        <v>207</v>
       </c>
       <c r="F62" t="n">
         <v>1.0</v>
       </c>
       <c r="G62" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H62" t="s">
         <v>20</v>
       </c>
       <c r="I62" t="n">
-        <v>60.0</v>
+        <v>70.0</v>
       </c>
       <c r="J62" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="K62" t="n">
         <v>44383.0</v>
       </c>
       <c r="L62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M62" t="s">
-        <v>24</v>
+        <v>175</v>
       </c>
       <c r="N62" t="s">
-        <v>70</v>
+        <v>202</v>
       </c>
       <c r="O62" t="n">
         <v>1.0</v>
       </c>
       <c r="P62" t="n">
-        <v>39.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B63" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C63" t="s">
-        <v>187</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>123</v>
+        <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="F63" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G63" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H63" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="I63" t="n">
         <v>0.0</v>
       </c>
       <c r="J63" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K63" t="n">
         <v>44383.0</v>
       </c>
       <c r="L63" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M63" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="N63" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="O63" t="n">
         <v>1.0</v>
       </c>
       <c r="P63" t="n">
-        <v>43.0</v>
+        <v>23.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>